<commit_message>
Update: Se Modifica Matriz De Calidad De Software
</commit_message>
<xml_diff>
--- a/6- VI_Trimestre/05- Matriz_Calidad_De_Software/01- Matriz_Calidad_De_Software.xlsx
+++ b/6- VI_Trimestre/05- Matriz_Calidad_De_Software/01- Matriz_Calidad_De_Software.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Andres_Olaya\Proyecto_Formativo\Kyukeisho_New\Kyukeisho_New\6- VI_Trimestre\05- Matriz_Calidad_De_Software\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10CA5B03-957F-47B0-BC42-2D9CB7B992B6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E446F8A-B338-4F70-B119-8F7AE9A407EF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{D58A99C2-3583-4B04-BA4C-07AC581D820A}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="74">
   <si>
     <t>Puntos Criticos</t>
   </si>
@@ -121,9 +121,6 @@
   </si>
   <si>
     <t>Casos De Uso Extendido</t>
-  </si>
-  <si>
-    <t>Control De Versiones</t>
   </si>
   <si>
     <t>Diseño</t>
@@ -358,7 +355,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="59">
+  <borders count="58">
     <border>
       <left/>
       <right/>
@@ -636,15 +633,6 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
       <bottom/>
       <diagonal/>
     </border>
@@ -1075,7 +1063,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="98">
+  <cellXfs count="100">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1092,38 +1080,38 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="33" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="34" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="34" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="37" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="35" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="35" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="38" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="36" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="24" xfId="3" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="2" fillId="4" borderId="36" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="2" fillId="4" borderId="27" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="25" xfId="3" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="2" fillId="4" borderId="37" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="2" fillId="4" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="26" xfId="3" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="2" fillId="4" borderId="27" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="2" fillId="4" borderId="26" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="23" xfId="3" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="2" fillId="4" borderId="39" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="2" fillId="4" borderId="38" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="30" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="31" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="31" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="32" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="32" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="33" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="2" fillId="4" borderId="27" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="2" fillId="4" borderId="29" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="31" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="4" borderId="26" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="2" fillId="4" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="30" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="31" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="32" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="33" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="27" xfId="3" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="28" xfId="3" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="29" xfId="3" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1133,54 +1121,96 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="4" borderId="30" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="2" fillId="4" borderId="24" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="4" borderId="29" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="2" fillId="4" borderId="39" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="2" fillId="4" borderId="29" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="4" borderId="40" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="2" fillId="4" borderId="30" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="2" fillId="4" borderId="39" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="2" fillId="4" borderId="42" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="4" borderId="38" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="2" fillId="4" borderId="41" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="2" fillId="4" borderId="22" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="4" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="4" borderId="27" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="4" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="4" borderId="27" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="4" borderId="27" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="4" borderId="26" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="4" borderId="38" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="4" borderId="36" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="165" fontId="2" fillId="4" borderId="39" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="4" borderId="37" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="4" borderId="40" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="4" borderId="48" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="2" fillId="4" borderId="51" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="2" fillId="4" borderId="54" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="2" fillId="4" borderId="56" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="2" fillId="4" borderId="47" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="2" fillId="4" borderId="50" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="2" fillId="4" borderId="53" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="2" fillId="4" borderId="55" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="22" xfId="3" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="2" fillId="4" borderId="22" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="33" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="34" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="2" fillId="5" borderId="34" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="40" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="40" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="2" fillId="5" borderId="40" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="5" borderId="44" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="2" fillId="5" borderId="40" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="5" borderId="40" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="46" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="48" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="49" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="51" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="52" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="54" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="56" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="57" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1215,51 +1245,9 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="47" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="49" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="50" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="22" xfId="3" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="2" fillId="4" borderId="22" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="57" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="58" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="34" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="35" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="2" fillId="5" borderId="35" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="41" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="41" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="2" fillId="5" borderId="41" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="5" borderId="45" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="2" fillId="5" borderId="41" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="5" borderId="41" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="52" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="53" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="55" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="40% - Énfasis3" xfId="3" builtinId="39"/>
@@ -1841,10 +1829,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7014F898-5058-4D1B-9637-B21A5C3439BD}">
-  <dimension ref="A1:I1048571"/>
+  <dimension ref="A1:I1048570"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1863,30 +1851,30 @@
     <row r="2" spans="1:7" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D2" s="4"/>
       <c r="E2" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F2" s="6"/>
       <c r="G2" s="20"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B3" s="64"/>
-      <c r="C3" s="65"/>
-      <c r="D3" s="66"/>
-      <c r="E3" s="67"/>
-      <c r="F3" s="68"/>
-      <c r="G3" s="41"/>
+      <c r="B3" s="82"/>
+      <c r="C3" s="83"/>
+      <c r="D3" s="84"/>
+      <c r="E3" s="85"/>
+      <c r="F3" s="86"/>
+      <c r="G3" s="40"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B4" s="7" t="s">
         <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="D4" s="69"/>
-      <c r="E4" s="70"/>
-      <c r="F4" s="71"/>
-      <c r="G4" s="41"/>
+        <v>60</v>
+      </c>
+      <c r="D4" s="87"/>
+      <c r="E4" s="88"/>
+      <c r="F4" s="89"/>
+      <c r="G4" s="40"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B5" s="7" t="s">
@@ -1895,10 +1883,10 @@
       <c r="C5" s="8">
         <v>1803170</v>
       </c>
-      <c r="D5" s="69"/>
-      <c r="E5" s="70"/>
-      <c r="F5" s="71"/>
-      <c r="G5" s="41"/>
+      <c r="D5" s="87"/>
+      <c r="E5" s="88"/>
+      <c r="F5" s="89"/>
+      <c r="G5" s="40"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B6" s="36" t="s">
@@ -1907,10 +1895,10 @@
       <c r="C6" s="8">
         <v>1</v>
       </c>
-      <c r="D6" s="69"/>
-      <c r="E6" s="70"/>
-      <c r="F6" s="71"/>
-      <c r="G6" s="41"/>
+      <c r="D6" s="87"/>
+      <c r="E6" s="88"/>
+      <c r="F6" s="89"/>
+      <c r="G6" s="40"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B7" s="7" t="s">
@@ -1919,10 +1907,10 @@
       <c r="C7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="69"/>
-      <c r="E7" s="70"/>
-      <c r="F7" s="71"/>
-      <c r="G7" s="41"/>
+      <c r="D7" s="87"/>
+      <c r="E7" s="88"/>
+      <c r="F7" s="89"/>
+      <c r="G7" s="40"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B8" s="7" t="s">
@@ -1931,10 +1919,10 @@
       <c r="C8" s="9">
         <v>43500</v>
       </c>
-      <c r="D8" s="69"/>
-      <c r="E8" s="70"/>
-      <c r="F8" s="71"/>
-      <c r="G8" s="41"/>
+      <c r="D8" s="87"/>
+      <c r="E8" s="88"/>
+      <c r="F8" s="89"/>
+      <c r="G8" s="40"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B9" s="36" t="s">
@@ -1943,10 +1931,10 @@
       <c r="C9" s="9">
         <v>44000</v>
       </c>
-      <c r="D9" s="69"/>
-      <c r="E9" s="70"/>
-      <c r="F9" s="71"/>
-      <c r="G9" s="41"/>
+      <c r="D9" s="87"/>
+      <c r="E9" s="88"/>
+      <c r="F9" s="89"/>
+      <c r="G9" s="40"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B10" s="7" t="s">
@@ -1955,46 +1943,46 @@
       <c r="C10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="72"/>
-      <c r="E10" s="73"/>
-      <c r="F10" s="74"/>
-      <c r="G10" s="41"/>
+      <c r="D10" s="90"/>
+      <c r="E10" s="91"/>
+      <c r="F10" s="92"/>
+      <c r="G10" s="40"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B11" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="75" t="s">
+      <c r="C11" s="93" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="76"/>
-      <c r="E11" s="76"/>
-      <c r="F11" s="77"/>
-      <c r="G11" s="41"/>
+      <c r="D11" s="94"/>
+      <c r="E11" s="94"/>
+      <c r="F11" s="95"/>
+      <c r="G11" s="40"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B12" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="78" t="s">
+      <c r="C12" s="96" t="s">
         <v>13</v>
       </c>
-      <c r="D12" s="76"/>
-      <c r="E12" s="76"/>
-      <c r="F12" s="77"/>
-      <c r="G12" s="41"/>
+      <c r="D12" s="94"/>
+      <c r="E12" s="94"/>
+      <c r="F12" s="95"/>
+      <c r="G12" s="40"/>
     </row>
     <row r="13" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="59" t="s">
+      <c r="C13" s="77" t="s">
         <v>15</v>
       </c>
-      <c r="D13" s="60"/>
-      <c r="E13" s="60"/>
-      <c r="F13" s="61"/>
-      <c r="G13" s="41"/>
+      <c r="D13" s="78"/>
+      <c r="E13" s="78"/>
+      <c r="F13" s="79"/>
+      <c r="G13" s="40"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="20"/>
@@ -2002,35 +1990,35 @@
       <c r="C15" s="3"/>
     </row>
     <row r="17" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D17" s="62" t="s">
+      <c r="D17" s="80" t="s">
+        <v>62</v>
+      </c>
+      <c r="E17" s="81"/>
+      <c r="F17" s="81"/>
+      <c r="G17" s="81"/>
+      <c r="H17" s="81"/>
+    </row>
+    <row r="18" spans="2:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="50" t="s">
+        <v>61</v>
+      </c>
+      <c r="C18" s="51" t="s">
+        <v>17</v>
+      </c>
+      <c r="D18" s="51" t="s">
         <v>63</v>
       </c>
-      <c r="E17" s="63"/>
-      <c r="F17" s="63"/>
-      <c r="G17" s="63"/>
-      <c r="H17" s="63"/>
-    </row>
-    <row r="18" spans="2:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="51" t="s">
-        <v>62</v>
-      </c>
-      <c r="C18" s="52" t="s">
-        <v>17</v>
-      </c>
-      <c r="D18" s="52" t="s">
-        <v>64</v>
-      </c>
-      <c r="E18" s="53" t="s">
+      <c r="E18" s="52" t="s">
+        <v>66</v>
+      </c>
+      <c r="F18" s="52" t="s">
         <v>67</v>
       </c>
-      <c r="F18" s="53" t="s">
+      <c r="G18" s="52" t="s">
         <v>68</v>
       </c>
-      <c r="G18" s="53" t="s">
-        <v>69</v>
-      </c>
-      <c r="H18" s="54" t="s">
-        <v>66</v>
+      <c r="H18" s="53" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="19" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2045,7 +2033,7 @@
       <c r="H19" s="14"/>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B20" s="79">
+      <c r="B20" s="69">
         <v>1</v>
       </c>
       <c r="C20" s="15" t="s">
@@ -2063,12 +2051,13 @@
       <c r="G20" s="16">
         <v>0.01</v>
       </c>
-      <c r="H20" s="55">
+      <c r="H20" s="54">
         <v>0.05</v>
       </c>
+      <c r="I20" s="97"/>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B21" s="79"/>
+      <c r="B21" s="69"/>
       <c r="C21" s="18" t="s">
         <v>20</v>
       </c>
@@ -2084,12 +2073,13 @@
       <c r="G21" s="16">
         <v>0.05</v>
       </c>
-      <c r="H21" s="55">
+      <c r="H21" s="54">
         <v>0.05</v>
       </c>
+      <c r="I21" s="97"/>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B22" s="79"/>
+      <c r="B22" s="69"/>
       <c r="C22" s="18" t="s">
         <v>21</v>
       </c>
@@ -2105,12 +2095,13 @@
       <c r="G22" s="16">
         <v>0.05</v>
       </c>
-      <c r="H22" s="55">
+      <c r="H22" s="54">
         <v>0.05</v>
       </c>
+      <c r="I22" s="97"/>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B23" s="79"/>
+      <c r="B23" s="69"/>
       <c r="C23" s="18" t="s">
         <v>22</v>
       </c>
@@ -2126,12 +2117,13 @@
       <c r="G23" s="16">
         <v>0.05</v>
       </c>
-      <c r="H23" s="55">
+      <c r="H23" s="54">
         <v>0.02</v>
       </c>
+      <c r="I23" s="97"/>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B24" s="80"/>
+      <c r="B24" s="70"/>
       <c r="C24" s="18" t="s">
         <v>23</v>
       </c>
@@ -2147,13 +2139,13 @@
       <c r="G24" s="16">
         <v>0.33</v>
       </c>
-      <c r="H24" s="55">
+      <c r="H24" s="54">
         <v>0.02</v>
       </c>
-      <c r="I24" s="20"/>
+      <c r="I24" s="98"/>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B25" s="81">
+      <c r="B25" s="71">
         <v>2</v>
       </c>
       <c r="C25" s="18" t="s">
@@ -2171,13 +2163,13 @@
       <c r="G25" s="16">
         <v>0.01</v>
       </c>
-      <c r="H25" s="55">
-        <v>0.2</v>
-      </c>
-      <c r="I25" s="20"/>
+      <c r="H25" s="54">
+        <v>0.2</v>
+      </c>
+      <c r="I25" s="98"/>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B26" s="79"/>
+      <c r="B26" s="69"/>
       <c r="C26" s="18" t="s">
         <v>25</v>
       </c>
@@ -2193,13 +2185,13 @@
       <c r="G26" s="16">
         <v>0.05</v>
       </c>
-      <c r="H26" s="55">
+      <c r="H26" s="54">
         <v>0.05</v>
       </c>
-      <c r="I26" s="20"/>
+      <c r="I26" s="98"/>
     </row>
     <row r="27" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B27" s="79"/>
+      <c r="B27" s="69"/>
       <c r="C27" s="18" t="s">
         <v>26</v>
       </c>
@@ -2215,12 +2207,13 @@
       <c r="G27" s="16">
         <v>0.05</v>
       </c>
-      <c r="H27" s="55">
-        <v>0.1</v>
-      </c>
+      <c r="H27" s="54">
+        <v>0.1</v>
+      </c>
+      <c r="I27" s="97"/>
     </row>
     <row r="28" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B28" s="79"/>
+      <c r="B28" s="69"/>
       <c r="C28" s="18" t="s">
         <v>27</v>
       </c>
@@ -2236,12 +2229,13 @@
       <c r="G28" s="16">
         <v>0.05</v>
       </c>
-      <c r="H28" s="55">
-        <v>0.2</v>
-      </c>
+      <c r="H28" s="54">
+        <v>0.26</v>
+      </c>
+      <c r="I28" s="97"/>
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B29" s="79"/>
+      <c r="B29" s="69"/>
       <c r="C29" s="18" t="s">
         <v>28</v>
       </c>
@@ -2257,596 +2251,599 @@
       <c r="G29" s="16">
         <v>0.05</v>
       </c>
-      <c r="H29" s="55">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B30" s="79"/>
+      <c r="H29" s="54">
+        <v>0.1</v>
+      </c>
+      <c r="I29" s="97"/>
+    </row>
+    <row r="30" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="69"/>
       <c r="C30" s="18" t="s">
         <v>29</v>
       </c>
       <c r="D30" s="17">
-        <v>0.1</v>
+        <v>0.11</v>
       </c>
       <c r="E30" s="17">
         <v>0</v>
       </c>
       <c r="F30" s="16">
-        <v>0.11</v>
+        <v>0.12</v>
       </c>
       <c r="G30" s="16">
-        <v>0.1</v>
-      </c>
-      <c r="H30" s="55">
+        <v>0.2</v>
+      </c>
+      <c r="H30" s="54">
         <v>0.05</v>
       </c>
+      <c r="I30" s="97"/>
     </row>
     <row r="31" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="79"/>
-      <c r="C31" s="21" t="s">
+      <c r="B31" s="63" t="s">
+        <v>64</v>
+      </c>
+      <c r="C31" s="64"/>
+      <c r="D31" s="67">
+        <f>SUM(D20:D30)</f>
+        <v>0.95</v>
+      </c>
+      <c r="E31" s="67">
+        <f>SUM(E20:E30)</f>
+        <v>0</v>
+      </c>
+      <c r="F31" s="68">
+        <f>SUM(F20:F30)</f>
+        <v>0.95</v>
+      </c>
+      <c r="G31" s="68">
+        <f>SUM(G20:G30)</f>
+        <v>0.90000000000000013</v>
+      </c>
+      <c r="H31" s="68">
+        <f>SUM(H20:H30)</f>
+        <v>0.95000000000000007</v>
+      </c>
+      <c r="I31" s="99"/>
+    </row>
+    <row r="32" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="23"/>
+      <c r="C32" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="D31" s="38">
+      <c r="D32" s="24"/>
+      <c r="E32" s="24"/>
+      <c r="F32" s="24"/>
+      <c r="G32" s="24"/>
+      <c r="H32" s="26"/>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B33" s="72">
+        <v>3</v>
+      </c>
+      <c r="C33" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="D33" s="17">
+        <v>0.05</v>
+      </c>
+      <c r="E33" s="45" t="s">
+        <v>69</v>
+      </c>
+      <c r="F33" s="48" t="s">
+        <v>69</v>
+      </c>
+      <c r="G33" s="49" t="s">
+        <v>69</v>
+      </c>
+      <c r="H33" s="55">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B34" s="73"/>
+      <c r="C34" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="D34" s="17">
+        <v>0.25</v>
+      </c>
+      <c r="E34" s="17">
+        <v>0.35</v>
+      </c>
+      <c r="F34" s="27">
+        <v>0.25</v>
+      </c>
+      <c r="G34" s="41">
+        <v>0.45</v>
+      </c>
+      <c r="H34" s="56">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B35" s="73"/>
+      <c r="C35" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="D35" s="17">
+        <v>0.2</v>
+      </c>
+      <c r="E35" s="17">
+        <v>0.2</v>
+      </c>
+      <c r="F35" s="27">
+        <v>0.3</v>
+      </c>
+      <c r="G35" s="41">
+        <v>0.2</v>
+      </c>
+      <c r="H35" s="56">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B36" s="73"/>
+      <c r="C36" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="D36" s="17">
         <v>0.01</v>
       </c>
-      <c r="E31" s="37">
-        <v>0</v>
-      </c>
-      <c r="F31" s="39">
+      <c r="E36" s="45" t="s">
+        <v>69</v>
+      </c>
+      <c r="F36" s="46" t="s">
+        <v>69</v>
+      </c>
+      <c r="G36" s="47" t="s">
+        <v>70</v>
+      </c>
+      <c r="H36" s="56">
         <v>0.01</v>
       </c>
-      <c r="G31" s="39">
-        <v>0.15</v>
-      </c>
-      <c r="H31" s="56">
-        <v>0.06</v>
-      </c>
-    </row>
-    <row r="32" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="89" t="s">
-        <v>65</v>
-      </c>
-      <c r="C32" s="90"/>
-      <c r="D32" s="93">
-        <f>SUM(D20:D31)</f>
-        <v>0.95</v>
-      </c>
-      <c r="E32" s="93">
-        <f>SUM(E20:E31)</f>
-        <v>0</v>
-      </c>
-      <c r="F32" s="94">
-        <f>SUM(F20:F31)</f>
-        <v>0.95</v>
-      </c>
-      <c r="G32" s="94">
-        <f>SUM(G20:G31)</f>
-        <v>0.95000000000000018</v>
-      </c>
-      <c r="H32" s="94">
-        <f>SUM(H20:H31)</f>
-        <v>0.95</v>
-      </c>
-    </row>
-    <row r="33" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="23"/>
-      <c r="C33" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="D33" s="24"/>
-      <c r="E33" s="24"/>
-      <c r="F33" s="24"/>
-      <c r="G33" s="24"/>
-      <c r="H33" s="26"/>
-    </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B34" s="95">
-        <v>3</v>
-      </c>
-      <c r="C34" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="D34" s="17">
-        <v>0.05</v>
-      </c>
-      <c r="E34" s="46" t="s">
-        <v>70</v>
-      </c>
-      <c r="F34" s="49" t="s">
-        <v>70</v>
-      </c>
-      <c r="G34" s="50" t="s">
-        <v>70</v>
-      </c>
-      <c r="H34" s="56">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B35" s="96"/>
-      <c r="C35" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="D35" s="17">
-        <v>0.25</v>
-      </c>
-      <c r="E35" s="17">
-        <v>0.35</v>
-      </c>
-      <c r="F35" s="27">
-        <v>0.25</v>
-      </c>
-      <c r="G35" s="42">
-        <v>0.45</v>
-      </c>
-      <c r="H35" s="57">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B36" s="96"/>
-      <c r="C36" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="D36" s="17">
-        <v>0.2</v>
-      </c>
-      <c r="E36" s="17">
-        <v>0.2</v>
-      </c>
-      <c r="F36" s="27">
-        <v>0.3</v>
-      </c>
-      <c r="G36" s="42">
-        <v>0.2</v>
-      </c>
-      <c r="H36" s="57">
-        <v>0.3</v>
-      </c>
     </row>
     <row r="37" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B37" s="96"/>
+      <c r="B37" s="73"/>
       <c r="C37" s="18" t="s">
         <v>34</v>
       </c>
       <c r="D37" s="17">
-        <v>0.01</v>
-      </c>
-      <c r="E37" s="46" t="s">
-        <v>70</v>
-      </c>
-      <c r="F37" s="47" t="s">
-        <v>70</v>
-      </c>
-      <c r="G37" s="48" t="s">
-        <v>71</v>
-      </c>
-      <c r="H37" s="57">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B38" s="96"/>
-      <c r="C38" s="18" t="s">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="E37" s="17">
+        <v>0.1</v>
+      </c>
+      <c r="F37" s="27">
+        <v>0.2</v>
+      </c>
+      <c r="G37" s="41">
+        <v>0.1</v>
+      </c>
+      <c r="H37" s="56">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="38" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B38" s="74"/>
+      <c r="C38" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="D38" s="17">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="E38" s="17">
-        <v>0.1</v>
-      </c>
-      <c r="F38" s="27">
-        <v>0.2</v>
-      </c>
-      <c r="G38" s="42">
-        <v>0.1</v>
-      </c>
-      <c r="H38" s="57">
-        <v>0.2</v>
+      <c r="D38" s="39">
+        <v>0.3</v>
+      </c>
+      <c r="E38" s="39">
+        <v>0.3</v>
+      </c>
+      <c r="F38" s="41">
+        <v>0.2</v>
+      </c>
+      <c r="G38" s="41">
+        <v>0.2</v>
+      </c>
+      <c r="H38" s="56">
+        <v>0.09</v>
       </c>
     </row>
     <row r="39" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="97"/>
-      <c r="C39" s="21" t="s">
+      <c r="B39" s="63" t="s">
+        <v>64</v>
+      </c>
+      <c r="C39" s="64"/>
+      <c r="D39" s="65">
+        <f>SUM(D33:D38)</f>
+        <v>0.95</v>
+      </c>
+      <c r="E39" s="65">
+        <f>SUM(E33:E38)</f>
+        <v>0.95</v>
+      </c>
+      <c r="F39" s="65">
+        <f>SUM(F33:F38)</f>
+        <v>0.95</v>
+      </c>
+      <c r="G39" s="65">
+        <f>SUM(G33:G38)</f>
+        <v>0.95</v>
+      </c>
+      <c r="H39" s="65">
+        <f>SUM(H33:H38)</f>
+        <v>0.94999999999999984</v>
+      </c>
+    </row>
+    <row r="40" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B40" s="29"/>
+      <c r="C40" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="D39" s="40">
-        <v>0.3</v>
-      </c>
-      <c r="E39" s="40">
-        <v>0.3</v>
-      </c>
-      <c r="F39" s="42">
-        <v>0.2</v>
-      </c>
-      <c r="G39" s="42">
-        <v>0.2</v>
-      </c>
-      <c r="H39" s="57">
-        <v>0.09</v>
-      </c>
-    </row>
-    <row r="40" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="89" t="s">
-        <v>65</v>
-      </c>
-      <c r="C40" s="90"/>
-      <c r="D40" s="91">
-        <f>SUM(D34:D39)</f>
-        <v>0.95</v>
-      </c>
-      <c r="E40" s="91">
-        <f>SUM(E34:E39)</f>
-        <v>0.95</v>
-      </c>
-      <c r="F40" s="91">
-        <f>SUM(F34:F39)</f>
-        <v>0.95</v>
-      </c>
-      <c r="G40" s="91">
-        <f>SUM(G34:G39)</f>
-        <v>0.95</v>
-      </c>
-      <c r="H40" s="91">
-        <f>SUM(H34:H39)</f>
-        <v>0.94999999999999984</v>
-      </c>
-    </row>
-    <row r="41" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="29"/>
-      <c r="C41" s="25" t="s">
-        <v>37</v>
-      </c>
-      <c r="D41" s="30"/>
-      <c r="E41" s="30"/>
-      <c r="F41" s="30"/>
-      <c r="G41" s="30"/>
-      <c r="H41" s="31"/>
+      <c r="D40" s="30"/>
+      <c r="E40" s="30"/>
+      <c r="F40" s="30"/>
+      <c r="G40" s="30"/>
+      <c r="H40" s="31"/>
+    </row>
+    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B41" s="72">
+        <v>4</v>
+      </c>
+      <c r="C41" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="D41" s="44">
+        <v>0.2</v>
+      </c>
+      <c r="E41" s="44">
+        <v>0.1</v>
+      </c>
+      <c r="F41" s="38">
+        <v>0.05</v>
+      </c>
+      <c r="G41" s="38">
+        <v>0.1</v>
+      </c>
+      <c r="H41" s="55">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="42" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B42" s="95">
-        <v>4</v>
-      </c>
-      <c r="C42" s="15" t="s">
+      <c r="B42" s="73"/>
+      <c r="C42" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="D42" s="45">
-        <v>0.2</v>
-      </c>
-      <c r="E42" s="45">
-        <v>0.1</v>
-      </c>
-      <c r="F42" s="39">
+      <c r="D42" s="43">
+        <v>0.15</v>
+      </c>
+      <c r="E42" s="43">
+        <v>0.2</v>
+      </c>
+      <c r="F42" s="22">
         <v>0.05</v>
       </c>
-      <c r="G42" s="39">
-        <v>0.1</v>
+      <c r="G42" s="22">
+        <v>0.28999999999999998</v>
       </c>
       <c r="H42" s="56">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="43" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B43" s="96"/>
+      <c r="B43" s="73"/>
       <c r="C43" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="D43" s="44">
-        <v>0.15</v>
+      <c r="D43" s="43">
+        <v>0.1</v>
       </c>
       <c r="E43" s="44">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="F43" s="22">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="G43" s="22">
-        <v>0.28999999999999998</v>
-      </c>
-      <c r="H43" s="57">
-        <v>0.2</v>
+        <v>0.2</v>
+      </c>
+      <c r="H43" s="56">
+        <v>0.1</v>
       </c>
     </row>
     <row r="44" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B44" s="96"/>
+      <c r="B44" s="73"/>
       <c r="C44" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="D44" s="44">
-        <v>0.1</v>
-      </c>
-      <c r="E44" s="45">
-        <v>0.1</v>
+      <c r="D44" s="43">
+        <v>0.4</v>
+      </c>
+      <c r="E44" s="43">
+        <v>0.35</v>
       </c>
       <c r="F44" s="22">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="G44" s="22">
-        <v>0.2</v>
-      </c>
-      <c r="H44" s="57">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="45" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B45" s="96"/>
-      <c r="C45" s="18" t="s">
+        <v>0.35</v>
+      </c>
+      <c r="H44" s="56">
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="45" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B45" s="74"/>
+      <c r="C45" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="D45" s="44">
-        <v>0.4</v>
-      </c>
-      <c r="E45" s="44">
-        <v>0.35</v>
+      <c r="D45" s="39">
+        <v>0.1</v>
+      </c>
+      <c r="E45" s="39">
+        <v>0.2</v>
       </c>
       <c r="F45" s="22">
-        <v>0.1</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="G45" s="22">
-        <v>0.35</v>
-      </c>
-      <c r="H45" s="57">
-        <v>0.45</v>
+        <v>0.01</v>
+      </c>
+      <c r="H45" s="56">
+        <v>0.1</v>
       </c>
     </row>
     <row r="46" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B46" s="97"/>
-      <c r="C46" s="21" t="s">
+      <c r="B46" s="63" t="s">
+        <v>64</v>
+      </c>
+      <c r="C46" s="64"/>
+      <c r="D46" s="65">
+        <f>SUM(D41:D45)</f>
+        <v>0.95</v>
+      </c>
+      <c r="E46" s="65">
+        <f>SUM(E41:E45)</f>
+        <v>0.95</v>
+      </c>
+      <c r="F46" s="66">
+        <f>SUM(F41:F45)</f>
+        <v>0.95000000000000007</v>
+      </c>
+      <c r="G46" s="65">
+        <f>SUM(G41:G45)</f>
+        <v>0.95000000000000007</v>
+      </c>
+      <c r="H46" s="65">
+        <f>SUM(H41:H45)</f>
+        <v>0.95000000000000007</v>
+      </c>
+    </row>
+    <row r="47" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B47" s="29"/>
+      <c r="C47" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="D46" s="40">
-        <v>0.1</v>
-      </c>
-      <c r="E46" s="40">
-        <v>0.2</v>
-      </c>
-      <c r="F46" s="22">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="G46" s="22">
-        <v>0.01</v>
-      </c>
-      <c r="H46" s="57">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="47" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B47" s="89" t="s">
-        <v>65</v>
-      </c>
-      <c r="C47" s="90"/>
-      <c r="D47" s="91">
-        <f>SUM(D42:D46)</f>
-        <v>0.95</v>
-      </c>
-      <c r="E47" s="91">
-        <f>SUM(E42:E46)</f>
-        <v>0.95</v>
-      </c>
-      <c r="F47" s="92">
-        <f>SUM(F42:F46)</f>
-        <v>0.95000000000000007</v>
-      </c>
-      <c r="G47" s="91">
-        <f>SUM(G42:G46)</f>
-        <v>0.95000000000000007</v>
-      </c>
-      <c r="H47" s="91">
-        <f>SUM(H42:H46)</f>
-        <v>0.95000000000000007</v>
-      </c>
-    </row>
-    <row r="48" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B48" s="29"/>
-      <c r="C48" s="25" t="s">
+      <c r="D47" s="30"/>
+      <c r="E47" s="30"/>
+      <c r="F47" s="30"/>
+      <c r="G47" s="30"/>
+      <c r="H47" s="31"/>
+    </row>
+    <row r="48" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B48" s="72">
+        <v>5</v>
+      </c>
+      <c r="C48" s="32" t="s">
         <v>44</v>
       </c>
-      <c r="D48" s="30"/>
-      <c r="E48" s="30"/>
-      <c r="F48" s="30"/>
-      <c r="G48" s="30"/>
-      <c r="H48" s="31"/>
+      <c r="D48" s="42">
+        <v>0.2</v>
+      </c>
+      <c r="E48" s="42">
+        <v>0.2</v>
+      </c>
+      <c r="F48" s="28">
+        <v>0.2</v>
+      </c>
+      <c r="G48" s="28">
+        <v>0.18</v>
+      </c>
+      <c r="H48" s="56">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="49" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B49" s="95">
-        <v>5</v>
-      </c>
-      <c r="C49" s="32" t="s">
+      <c r="B49" s="73"/>
+      <c r="C49" s="18" t="s">
         <v>45</v>
       </c>
       <c r="D49" s="43">
-        <v>0.2</v>
-      </c>
-      <c r="E49" s="43">
-        <v>0.2</v>
+        <v>0.1</v>
+      </c>
+      <c r="E49" s="44">
+        <v>0.08</v>
       </c>
       <c r="F49" s="28">
-        <v>0.2</v>
+        <v>0.05</v>
       </c>
       <c r="G49" s="28">
-        <v>0.18</v>
-      </c>
-      <c r="H49" s="57">
+        <v>0.2</v>
+      </c>
+      <c r="H49" s="56">
         <v>0.1</v>
       </c>
     </row>
     <row r="50" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B50" s="96"/>
+      <c r="B50" s="73"/>
       <c r="C50" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="D50" s="44">
-        <v>0.1</v>
-      </c>
-      <c r="E50" s="45">
-        <v>0.08</v>
+      <c r="D50" s="43">
+        <v>0.15</v>
+      </c>
+      <c r="E50" s="44">
+        <v>0.2</v>
       </c>
       <c r="F50" s="28">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="G50" s="28">
-        <v>0.2</v>
-      </c>
-      <c r="H50" s="57">
+        <v>0.1</v>
+      </c>
+      <c r="H50" s="56">
         <v>0.1</v>
       </c>
     </row>
     <row r="51" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B51" s="96"/>
+      <c r="B51" s="73"/>
       <c r="C51" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="D51" s="44">
-        <v>0.15</v>
-      </c>
-      <c r="E51" s="45">
-        <v>0.2</v>
+      <c r="D51" s="43">
+        <v>0.48</v>
+      </c>
+      <c r="E51" s="43">
+        <v>0.45</v>
       </c>
       <c r="F51" s="28">
-        <v>0.2</v>
+        <v>0.05</v>
       </c>
       <c r="G51" s="28">
-        <v>0.1</v>
-      </c>
-      <c r="H51" s="57">
-        <v>0.1</v>
+        <v>0.45</v>
+      </c>
+      <c r="H51" s="56">
+        <v>0.45</v>
       </c>
     </row>
     <row r="52" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B52" s="96"/>
+      <c r="B52" s="73"/>
       <c r="C52" s="18" t="s">
         <v>48</v>
       </c>
       <c r="D52" s="44">
-        <v>0.48</v>
+        <v>0.01</v>
       </c>
       <c r="E52" s="44">
-        <v>0.45</v>
+        <v>0.01</v>
       </c>
       <c r="F52" s="28">
-        <v>0.05</v>
+        <v>0.35</v>
       </c>
       <c r="G52" s="28">
-        <v>0.45</v>
-      </c>
-      <c r="H52" s="57">
-        <v>0.45</v>
-      </c>
-    </row>
-    <row r="53" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B53" s="96"/>
-      <c r="C53" s="18" t="s">
+        <v>0.01</v>
+      </c>
+      <c r="H52" s="56">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="53" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B53" s="74"/>
+      <c r="C53" s="33" t="s">
         <v>49</v>
       </c>
-      <c r="D53" s="45">
+      <c r="D53" s="39">
         <v>0.01</v>
       </c>
-      <c r="E53" s="45">
+      <c r="E53" s="39">
         <v>0.01</v>
       </c>
       <c r="F53" s="28">
-        <v>0.35</v>
+        <v>0.1</v>
       </c>
       <c r="G53" s="28">
         <v>0.01</v>
       </c>
-      <c r="H53" s="57">
+      <c r="H53" s="56">
         <v>0.1</v>
       </c>
     </row>
     <row r="54" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B54" s="97"/>
-      <c r="C54" s="33" t="s">
+      <c r="B54" s="63" t="s">
+        <v>64</v>
+      </c>
+      <c r="C54" s="64"/>
+      <c r="D54" s="65">
+        <f>SUM(D48:D53)</f>
+        <v>0.95000000000000007</v>
+      </c>
+      <c r="E54" s="65">
+        <f>SUM(E48:E53)</f>
+        <v>0.95000000000000007</v>
+      </c>
+      <c r="F54" s="65">
+        <f>SUM(F48:F53)</f>
+        <v>0.95</v>
+      </c>
+      <c r="G54" s="65">
+        <f>SUM(G48:G53)</f>
+        <v>0.95</v>
+      </c>
+      <c r="H54" s="65">
+        <f>SUM(H48:H53)</f>
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="55" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B55" s="29"/>
+      <c r="C55" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="D54" s="40">
-        <v>0.01</v>
-      </c>
-      <c r="E54" s="40">
-        <v>0.01</v>
-      </c>
-      <c r="F54" s="28">
-        <v>0.1</v>
-      </c>
-      <c r="G54" s="28">
-        <v>0.01</v>
-      </c>
-      <c r="H54" s="57">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="55" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B55" s="89" t="s">
-        <v>65</v>
-      </c>
-      <c r="C55" s="90"/>
-      <c r="D55" s="91">
-        <f>SUM(D49:D54)</f>
-        <v>0.95000000000000007</v>
-      </c>
-      <c r="E55" s="91">
-        <f>SUM(E49:E54)</f>
-        <v>0.95000000000000007</v>
-      </c>
-      <c r="F55" s="91">
-        <f>SUM(F49:F54)</f>
-        <v>0.95</v>
-      </c>
-      <c r="G55" s="91">
-        <f>SUM(G49:G54)</f>
-        <v>0.95</v>
-      </c>
-      <c r="H55" s="91">
-        <f>SUM(H49:H54)</f>
-        <v>0.95</v>
-      </c>
-    </row>
-    <row r="56" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B56" s="29"/>
-      <c r="C56" s="12" t="s">
+      <c r="D55" s="30"/>
+      <c r="E55" s="30"/>
+      <c r="F55" s="30"/>
+      <c r="G55" s="30"/>
+      <c r="H55" s="31"/>
+    </row>
+    <row r="56" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B56" s="72">
+        <v>6</v>
+      </c>
+      <c r="C56" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="D56" s="30"/>
-      <c r="E56" s="30"/>
-      <c r="F56" s="30"/>
-      <c r="G56" s="30"/>
-      <c r="H56" s="31"/>
+      <c r="D56" s="42">
+        <v>0.1</v>
+      </c>
+      <c r="E56" s="42">
+        <v>0.1</v>
+      </c>
+      <c r="F56" s="17">
+        <v>0.1</v>
+      </c>
+      <c r="G56" s="37">
+        <v>0.1</v>
+      </c>
+      <c r="H56" s="56">
+        <v>0.15</v>
+      </c>
     </row>
     <row r="57" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B57" s="95">
-        <v>6</v>
-      </c>
-      <c r="C57" s="32" t="s">
+      <c r="B57" s="73"/>
+      <c r="C57" s="18" t="s">
         <v>52</v>
       </c>
       <c r="D57" s="43">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="E57" s="43">
         <v>0.1</v>
       </c>
-      <c r="F57" s="17">
-        <v>0.1</v>
-      </c>
-      <c r="G57" s="37">
-        <v>0.1</v>
-      </c>
-      <c r="H57" s="57">
+      <c r="F57" s="28">
+        <v>0.1</v>
+      </c>
+      <c r="G57" s="28">
+        <v>0.1</v>
+      </c>
+      <c r="H57" s="56">
         <v>0.15</v>
       </c>
     </row>
     <row r="58" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B58" s="96"/>
+      <c r="B58" s="73"/>
       <c r="C58" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="D58" s="44">
-        <v>0.2</v>
-      </c>
-      <c r="E58" s="44">
-        <v>0.1</v>
+      <c r="D58" s="43">
+        <v>0.2</v>
+      </c>
+      <c r="E58" s="43">
+        <v>0.2</v>
       </c>
       <c r="F58" s="28">
         <v>0.1</v>
@@ -2854,284 +2851,266 @@
       <c r="G58" s="28">
         <v>0.1</v>
       </c>
-      <c r="H58" s="57">
+      <c r="H58" s="56">
         <v>0.15</v>
       </c>
     </row>
     <row r="59" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B59" s="96"/>
+      <c r="B59" s="73"/>
       <c r="C59" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="D59" s="44">
-        <v>0.2</v>
-      </c>
-      <c r="E59" s="44">
-        <v>0.2</v>
+      <c r="D59" s="43">
+        <v>0.1</v>
+      </c>
+      <c r="E59" s="43">
+        <v>0.15</v>
       </c>
       <c r="F59" s="28">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="G59" s="28">
-        <v>0.1</v>
-      </c>
-      <c r="H59" s="57">
-        <v>0.15</v>
+        <v>0.05</v>
+      </c>
+      <c r="H59" s="56">
+        <v>0.1</v>
       </c>
     </row>
     <row r="60" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B60" s="96"/>
+      <c r="B60" s="73"/>
       <c r="C60" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="D60" s="44">
-        <v>0.1</v>
-      </c>
-      <c r="E60" s="44">
+      <c r="D60" s="43">
+        <v>0.1</v>
+      </c>
+      <c r="E60" s="43">
+        <v>0.2</v>
+      </c>
+      <c r="F60" s="28">
+        <v>0.1</v>
+      </c>
+      <c r="G60" s="28">
+        <v>0.1</v>
+      </c>
+      <c r="H60" s="56">
         <v>0.15</v>
       </c>
-      <c r="F60" s="28">
-        <v>0.05</v>
-      </c>
-      <c r="G60" s="28">
-        <v>0.05</v>
-      </c>
-      <c r="H60" s="57">
-        <v>0.1</v>
-      </c>
     </row>
     <row r="61" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B61" s="96"/>
+      <c r="B61" s="73"/>
       <c r="C61" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="D61" s="44">
-        <v>0.1</v>
-      </c>
-      <c r="E61" s="44">
-        <v>0.2</v>
+      <c r="D61" s="43">
+        <v>0.1</v>
+      </c>
+      <c r="E61" s="43">
+        <v>0.1</v>
       </c>
       <c r="F61" s="28">
-        <v>0.1</v>
+        <v>0.4</v>
       </c>
       <c r="G61" s="28">
         <v>0.1</v>
       </c>
-      <c r="H61" s="57">
+      <c r="H61" s="56">
         <v>0.15</v>
       </c>
     </row>
-    <row r="62" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B62" s="96"/>
-      <c r="C62" s="18" t="s">
+    <row r="62" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B62" s="74"/>
+      <c r="C62" s="33" t="s">
         <v>57</v>
       </c>
-      <c r="D62" s="44">
-        <v>0.1</v>
-      </c>
-      <c r="E62" s="44">
+      <c r="D62" s="39">
+        <v>0.15</v>
+      </c>
+      <c r="E62" s="39">
         <v>0.1</v>
       </c>
       <c r="F62" s="28">
+        <v>0.1</v>
+      </c>
+      <c r="G62" s="28">
         <v>0.4</v>
       </c>
-      <c r="G62" s="28">
-        <v>0.1</v>
-      </c>
-      <c r="H62" s="57">
+      <c r="H62" s="56">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="63" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B63" s="63" t="s">
+        <v>64</v>
+      </c>
+      <c r="C63" s="64"/>
+      <c r="D63" s="65">
+        <f>SUM(D56:D62)</f>
+        <v>0.95</v>
+      </c>
+      <c r="E63" s="65">
+        <f>SUM(E56:E62)</f>
+        <v>0.95</v>
+      </c>
+      <c r="F63" s="65">
+        <f>SUM(F56:F62)</f>
+        <v>0.95000000000000007</v>
+      </c>
+      <c r="G63" s="65">
+        <f>SUM(G56:G62)</f>
+        <v>0.95000000000000007</v>
+      </c>
+      <c r="H63" s="65">
+        <f>SUM(H56:H62)</f>
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="64" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B64" s="29"/>
+      <c r="C64" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="D64" s="30"/>
+      <c r="E64" s="30"/>
+      <c r="F64" s="30"/>
+      <c r="G64" s="30"/>
+      <c r="H64" s="31"/>
+    </row>
+    <row r="65" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B65" s="75">
+        <v>7</v>
+      </c>
+      <c r="C65" s="32" t="s">
+        <v>59</v>
+      </c>
+      <c r="D65" s="19">
         <v>0.15</v>
       </c>
-    </row>
-    <row r="63" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B63" s="97"/>
-      <c r="C63" s="33" t="s">
-        <v>58</v>
-      </c>
-      <c r="D63" s="40">
+      <c r="E65" s="19">
         <v>0.15</v>
       </c>
-      <c r="E63" s="40">
-        <v>0.1</v>
-      </c>
-      <c r="F63" s="28">
-        <v>0.1</v>
-      </c>
-      <c r="G63" s="28">
-        <v>0.4</v>
-      </c>
-      <c r="H63" s="57">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="64" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B64" s="89" t="s">
-        <v>65</v>
-      </c>
-      <c r="C64" s="90"/>
-      <c r="D64" s="91">
-        <f>SUM(D57:D63)</f>
+      <c r="F65" s="17">
+        <v>0.15</v>
+      </c>
+      <c r="G65" s="17">
+        <v>0.15</v>
+      </c>
+      <c r="H65" s="54">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="66" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B66" s="76"/>
+      <c r="C66" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="D66" s="59">
+        <v>0.2</v>
+      </c>
+      <c r="E66" s="19">
+        <v>0.2</v>
+      </c>
+      <c r="F66" s="19">
+        <v>0.2</v>
+      </c>
+      <c r="G66" s="19">
+        <v>0.2</v>
+      </c>
+      <c r="H66" s="57">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="67" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B67" s="76"/>
+      <c r="C67" s="33" t="s">
+        <v>16</v>
+      </c>
+      <c r="D67" s="59">
+        <v>0.2</v>
+      </c>
+      <c r="E67" s="59">
+        <v>0.2</v>
+      </c>
+      <c r="F67" s="22">
+        <v>0.2</v>
+      </c>
+      <c r="G67" s="22">
+        <v>0.2</v>
+      </c>
+      <c r="H67" s="56">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="68" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B68" s="76"/>
+      <c r="C68" s="58" t="s">
+        <v>71</v>
+      </c>
+      <c r="D68" s="59">
+        <v>0.2</v>
+      </c>
+      <c r="E68" s="59">
+        <v>0.2</v>
+      </c>
+      <c r="F68" s="22">
+        <v>0.2</v>
+      </c>
+      <c r="G68" s="22">
+        <v>0.2</v>
+      </c>
+      <c r="H68" s="56">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="69" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B69" s="76"/>
+      <c r="C69" s="33" t="s">
+        <v>72</v>
+      </c>
+      <c r="D69" s="28">
+        <v>0.2</v>
+      </c>
+      <c r="E69" s="28">
+        <v>0.2</v>
+      </c>
+      <c r="F69" s="22">
+        <v>0.2</v>
+      </c>
+      <c r="G69" s="22">
+        <v>0.2</v>
+      </c>
+      <c r="H69" s="56">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="70" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B70" s="60" t="s">
+        <v>64</v>
+      </c>
+      <c r="C70" s="61"/>
+      <c r="D70" s="62">
+        <f>SUM(D65:D69)</f>
         <v>0.95</v>
       </c>
-      <c r="E64" s="91">
-        <f>SUM(E57:E63)</f>
+      <c r="E70" s="62">
+        <f>SUM(E65:E69)</f>
         <v>0.95</v>
       </c>
-      <c r="F64" s="91">
-        <f>SUM(F57:F63)</f>
-        <v>0.95000000000000007</v>
-      </c>
-      <c r="G64" s="91">
-        <f>SUM(G57:G63)</f>
-        <v>0.95000000000000007</v>
-      </c>
-      <c r="H64" s="91">
-        <f>SUM(H57:H63)</f>
+      <c r="F70" s="62">
+        <f>SUM(F65:F69)</f>
         <v>0.95</v>
       </c>
-    </row>
-    <row r="65" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B65" s="29"/>
-      <c r="C65" s="25" t="s">
-        <v>59</v>
-      </c>
-      <c r="D65" s="30"/>
-      <c r="E65" s="30"/>
-      <c r="F65" s="30"/>
-      <c r="G65" s="30"/>
-      <c r="H65" s="31"/>
-    </row>
-    <row r="66" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B66" s="84">
-        <v>7</v>
-      </c>
-      <c r="C66" s="32" t="s">
-        <v>60</v>
-      </c>
-      <c r="D66" s="19">
-        <v>0.15</v>
-      </c>
-      <c r="E66" s="19">
-        <v>0.15</v>
-      </c>
-      <c r="F66" s="17">
-        <v>0.15</v>
-      </c>
-      <c r="G66" s="17">
-        <v>0.15</v>
-      </c>
-      <c r="H66" s="55">
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="67" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B67" s="85"/>
-      <c r="C67" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="D67" s="83">
-        <v>0.2</v>
-      </c>
-      <c r="E67" s="19">
-        <v>0.2</v>
-      </c>
-      <c r="F67" s="19">
-        <v>0.2</v>
-      </c>
-      <c r="G67" s="19">
-        <v>0.2</v>
-      </c>
-      <c r="H67" s="58">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="68" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B68" s="85"/>
-      <c r="C68" s="33" t="s">
-        <v>16</v>
-      </c>
-      <c r="D68" s="83">
-        <v>0.2</v>
-      </c>
-      <c r="E68" s="83">
-        <v>0.2</v>
-      </c>
-      <c r="F68" s="22">
-        <v>0.2</v>
-      </c>
-      <c r="G68" s="22">
-        <v>0.2</v>
-      </c>
-      <c r="H68" s="57">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="69" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B69" s="85"/>
-      <c r="C69" s="82" t="s">
-        <v>72</v>
-      </c>
-      <c r="D69" s="83">
-        <v>0.2</v>
-      </c>
-      <c r="E69" s="83">
-        <v>0.2</v>
-      </c>
-      <c r="F69" s="22">
-        <v>0.2</v>
-      </c>
-      <c r="G69" s="22">
-        <v>0.2</v>
-      </c>
-      <c r="H69" s="57">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="70" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B70" s="85"/>
-      <c r="C70" s="33" t="s">
-        <v>73</v>
-      </c>
-      <c r="D70" s="28">
-        <v>0.2</v>
-      </c>
-      <c r="E70" s="28">
-        <v>0.2</v>
-      </c>
-      <c r="F70" s="22">
-        <v>0.2</v>
-      </c>
-      <c r="G70" s="22">
-        <v>0.2</v>
-      </c>
-      <c r="H70" s="57">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="71" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B71" s="86" t="s">
-        <v>65</v>
-      </c>
-      <c r="C71" s="87"/>
-      <c r="D71" s="88">
-        <f>SUM(D66:D70)</f>
+      <c r="G70" s="62">
+        <f>SUM(G65:G69)</f>
         <v>0.95</v>
       </c>
-      <c r="E71" s="88">
-        <f>SUM(E66:E70)</f>
+      <c r="H70" s="62">
+        <f>SUM(H65:H69)</f>
         <v>0.95</v>
       </c>
-      <c r="F71" s="88">
-        <f>SUM(F66:F70)</f>
-        <v>0.95</v>
-      </c>
-      <c r="G71" s="88">
-        <f>SUM(G66:G70)</f>
-        <v>0.95</v>
-      </c>
-      <c r="H71" s="88">
-        <f>SUM(H66:H70)</f>
-        <v>0.95</v>
-      </c>
+    </row>
+    <row r="71" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B71" s="34"/>
     </row>
     <row r="72" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B72" s="34"/>
@@ -3376,27 +3355,24 @@
     <row r="152" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B152" s="34"/>
     </row>
-    <row r="153" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B153" s="34"/>
-    </row>
-    <row r="1048571" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D1048571" s="17"/>
+    <row r="1048570" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D1048570" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="B20:B24"/>
-    <mergeCell ref="B25:B31"/>
-    <mergeCell ref="B34:B39"/>
-    <mergeCell ref="B42:B46"/>
-    <mergeCell ref="B49:B54"/>
-    <mergeCell ref="B57:B63"/>
-    <mergeCell ref="B66:B70"/>
+    <mergeCell ref="B56:B62"/>
+    <mergeCell ref="B65:B69"/>
     <mergeCell ref="C13:F13"/>
     <mergeCell ref="D17:H17"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="D3:F10"/>
     <mergeCell ref="C11:F11"/>
     <mergeCell ref="C12:F12"/>
+    <mergeCell ref="B20:B24"/>
+    <mergeCell ref="B25:B30"/>
+    <mergeCell ref="B33:B38"/>
+    <mergeCell ref="B41:B45"/>
+    <mergeCell ref="B48:B53"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Update: Se Modifica Documento Matriz De Calidad
</commit_message>
<xml_diff>
--- a/6- VI_Trimestre/05- Matriz_Calidad_De_Software/01- Matriz_Calidad_De_Software.xlsx
+++ b/6- VI_Trimestre/05- Matriz_Calidad_De_Software/01- Matriz_Calidad_De_Software.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Andres_Olaya\Proyecto_Formativo\Kyukeisho_New\Kyukeisho_New\6- VI_Trimestre\05- Matriz_Calidad_De_Software\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E446F8A-B338-4F70-B119-8F7AE9A407EF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BEB2CAD-F3DF-4C4C-949D-F0AD5D2CDBFD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{D58A99C2-3583-4B04-BA4C-07AC581D820A}"/>
   </bookViews>
@@ -1187,15 +1187,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="2" fillId="5" borderId="40" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="46" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="48" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="49" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="51" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1245,9 +1239,15 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="46" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="48" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="49" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="40% - Énfasis3" xfId="3" builtinId="39"/>
@@ -1831,8 +1831,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7014F898-5058-4D1B-9637-B21A5C3439BD}">
   <dimension ref="A1:I1048570"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="I28" sqref="I28"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2033,7 +2033,7 @@
       <c r="H19" s="14"/>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B20" s="69">
+      <c r="B20" s="97">
         <v>1</v>
       </c>
       <c r="C20" s="15" t="s">
@@ -2043,7 +2043,7 @@
         <v>0.05</v>
       </c>
       <c r="E20" s="16">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="F20" s="16">
         <v>0.01</v>
@@ -2054,10 +2054,10 @@
       <c r="H20" s="54">
         <v>0.05</v>
       </c>
-      <c r="I20" s="97"/>
+      <c r="I20" s="69"/>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B21" s="69"/>
+      <c r="B21" s="97"/>
       <c r="C21" s="18" t="s">
         <v>20</v>
       </c>
@@ -2065,7 +2065,7 @@
         <v>0.1</v>
       </c>
       <c r="E21" s="16">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="F21" s="16">
         <v>0.1</v>
@@ -2076,10 +2076,10 @@
       <c r="H21" s="54">
         <v>0.05</v>
       </c>
-      <c r="I21" s="97"/>
+      <c r="I21" s="69"/>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B22" s="69"/>
+      <c r="B22" s="97"/>
       <c r="C22" s="18" t="s">
         <v>21</v>
       </c>
@@ -2087,7 +2087,7 @@
         <v>0.1</v>
       </c>
       <c r="E22" s="16">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="F22" s="16">
         <v>0.1</v>
@@ -2098,10 +2098,10 @@
       <c r="H22" s="54">
         <v>0.05</v>
       </c>
-      <c r="I22" s="97"/>
+      <c r="I22" s="69"/>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B23" s="69"/>
+      <c r="B23" s="97"/>
       <c r="C23" s="18" t="s">
         <v>22</v>
       </c>
@@ -2109,7 +2109,7 @@
         <v>0.02</v>
       </c>
       <c r="E23" s="16">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="F23" s="16">
         <v>0.01</v>
@@ -2120,10 +2120,10 @@
       <c r="H23" s="54">
         <v>0.02</v>
       </c>
-      <c r="I23" s="97"/>
+      <c r="I23" s="69"/>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B24" s="70"/>
+      <c r="B24" s="98"/>
       <c r="C24" s="18" t="s">
         <v>23</v>
       </c>
@@ -2131,7 +2131,7 @@
         <v>0.02</v>
       </c>
       <c r="E24" s="16">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="F24" s="16">
         <v>0.01</v>
@@ -2142,10 +2142,10 @@
       <c r="H24" s="54">
         <v>0.02</v>
       </c>
-      <c r="I24" s="98"/>
+      <c r="I24" s="70"/>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B25" s="71">
+      <c r="B25" s="99">
         <v>2</v>
       </c>
       <c r="C25" s="18" t="s">
@@ -2155,7 +2155,7 @@
         <v>0.1</v>
       </c>
       <c r="E25" s="17">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="F25" s="16">
         <v>0.05</v>
@@ -2166,10 +2166,10 @@
       <c r="H25" s="54">
         <v>0.2</v>
       </c>
-      <c r="I25" s="98"/>
+      <c r="I25" s="70"/>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B26" s="69"/>
+      <c r="B26" s="97"/>
       <c r="C26" s="18" t="s">
         <v>25</v>
       </c>
@@ -2177,7 +2177,7 @@
         <v>0.1</v>
       </c>
       <c r="E26" s="17">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="F26" s="16">
         <v>0.1</v>
@@ -2188,10 +2188,10 @@
       <c r="H26" s="54">
         <v>0.05</v>
       </c>
-      <c r="I26" s="98"/>
+      <c r="I26" s="70"/>
     </row>
     <row r="27" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B27" s="69"/>
+      <c r="B27" s="97"/>
       <c r="C27" s="18" t="s">
         <v>26</v>
       </c>
@@ -2199,7 +2199,7 @@
         <v>0.15</v>
       </c>
       <c r="E27" s="17">
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="F27" s="16">
         <v>0.15</v>
@@ -2210,10 +2210,10 @@
       <c r="H27" s="54">
         <v>0.1</v>
       </c>
-      <c r="I27" s="97"/>
+      <c r="I27" s="69"/>
     </row>
     <row r="28" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B28" s="69"/>
+      <c r="B28" s="97"/>
       <c r="C28" s="18" t="s">
         <v>27</v>
       </c>
@@ -2221,7 +2221,7 @@
         <v>0.1</v>
       </c>
       <c r="E28" s="17">
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="F28" s="16">
         <v>0.2</v>
@@ -2232,10 +2232,10 @@
       <c r="H28" s="54">
         <v>0.26</v>
       </c>
-      <c r="I28" s="97"/>
+      <c r="I28" s="69"/>
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B29" s="69"/>
+      <c r="B29" s="97"/>
       <c r="C29" s="18" t="s">
         <v>28</v>
       </c>
@@ -2243,7 +2243,7 @@
         <v>0.1</v>
       </c>
       <c r="E29" s="17">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="F29" s="16">
         <v>0.1</v>
@@ -2254,10 +2254,10 @@
       <c r="H29" s="54">
         <v>0.1</v>
       </c>
-      <c r="I29" s="97"/>
+      <c r="I29" s="69"/>
     </row>
     <row r="30" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="69"/>
+      <c r="B30" s="97"/>
       <c r="C30" s="18" t="s">
         <v>29</v>
       </c>
@@ -2265,7 +2265,7 @@
         <v>0.11</v>
       </c>
       <c r="E30" s="17">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="F30" s="16">
         <v>0.12</v>
@@ -2276,7 +2276,7 @@
       <c r="H30" s="54">
         <v>0.05</v>
       </c>
-      <c r="I30" s="97"/>
+      <c r="I30" s="69"/>
     </row>
     <row r="31" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B31" s="63" t="s">
@@ -2289,7 +2289,7 @@
       </c>
       <c r="E31" s="67">
         <f>SUM(E20:E30)</f>
-        <v>0</v>
+        <v>0.95000000000000007</v>
       </c>
       <c r="F31" s="68">
         <f>SUM(F20:F30)</f>
@@ -2303,7 +2303,7 @@
         <f>SUM(H20:H30)</f>
         <v>0.95000000000000007</v>
       </c>
-      <c r="I31" s="99"/>
+      <c r="I31" s="71"/>
     </row>
     <row r="32" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B32" s="23"/>
@@ -3374,6 +3374,90 @@
     <mergeCell ref="B41:B45"/>
     <mergeCell ref="B48:B53"/>
   </mergeCells>
+  <conditionalFormatting sqref="D20:D30">
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E20:H30">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D33:H38">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D41:H45">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D48:H53">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D56:H62">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D65:H69">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <drawing r:id="rId2"/>

</xml_diff>

<commit_message>
Create: Se Crea ISO 25000
</commit_message>
<xml_diff>
--- a/6- VI_Trimestre/05- Matriz_Calidad_De_Software/01- Matriz_Calidad_De_Software.xlsx
+++ b/6- VI_Trimestre/05- Matriz_Calidad_De_Software/01- Matriz_Calidad_De_Software.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Andres_Olaya\Proyecto_Formativo\Kyukeisho_New\Kyukeisho_New\6- VI_Trimestre\05- Matriz_Calidad_De_Software\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E816F36-230D-477B-8F6F-35DC6A2D50D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4973DD3-9809-4871-A2C9-FA45939D1A90}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{D58A99C2-3583-4B04-BA4C-07AC581D820A}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="79">
   <si>
     <t>Puntos Criticos</t>
   </si>
@@ -259,13 +259,23 @@
   </si>
   <si>
     <t>Cumplimiento Entregable</t>
+  </si>
+  <si>
+    <t>Peso Fase</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Pocentaje Por Fase</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="d/m/yyyy"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
   </numFmts>
@@ -760,40 +770,10 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
+      <left style="thin">
         <color indexed="64"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
         <color indexed="64"/>
       </right>
       <top style="medium">
@@ -816,19 +796,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="thin">
         <color indexed="64"/>
@@ -911,6 +878,32 @@
     </border>
     <border>
       <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color indexed="64"/>
       </left>
       <right/>
@@ -919,24 +912,79 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
       <right/>
       <top/>
-      <bottom style="thin">
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
+      <left/>
       <right/>
       <top style="thin">
         <color indexed="64"/>
       </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -948,6 +996,21 @@
         <color indexed="64"/>
       </right>
       <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -957,7 +1020,7 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="thin">
+      <right style="medium">
         <color indexed="64"/>
       </right>
       <top style="thin">
@@ -972,82 +1035,26 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="thin">
+      <right style="medium">
         <color indexed="64"/>
       </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="124">
+  <cellXfs count="150">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1065,35 +1072,20 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="33" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="34" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="34" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="37" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="35" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="24" xfId="3" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="2" fillId="4" borderId="36" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="2" fillId="4" borderId="34" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="2" fillId="4" borderId="27" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="25" xfId="3" applyFont="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="2" fillId="4" borderId="26" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="23" xfId="3" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="2" fillId="4" borderId="38" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="30" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="2" fillId="4" borderId="35" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="31" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="31" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="2" fillId="4" borderId="26" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="2" fillId="4" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="30" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="31" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="27" xfId="3" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="28" xfId="3" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1104,13 +1096,13 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="165" fontId="2" fillId="4" borderId="29" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="2" fillId="4" borderId="39" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="2" fillId="4" borderId="36" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="2" fillId="4" borderId="29" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="2" fillId="4" borderId="38" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="2" fillId="4" borderId="41" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="4" borderId="35" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="2" fillId="4" borderId="38" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="2" fillId="4" borderId="22" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1125,69 +1117,84 @@
     <xf numFmtId="165" fontId="2" fillId="4" borderId="26" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="4" borderId="38" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="4" borderId="35" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="4" borderId="34" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="165" fontId="2" fillId="4" borderId="36" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="4" borderId="39" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="22" xfId="3" applyFont="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="2" fillId="4" borderId="22" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="33" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="34" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="2" fillId="5" borderId="34" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="40" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="40" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="2" fillId="5" borderId="40" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="33" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="2" fillId="5" borderId="33" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="37" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="2" fillId="5" borderId="37" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="10" fontId="2" fillId="5" borderId="40" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="2" fillId="5" borderId="37" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="5" borderId="40" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="5" borderId="37" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="4" borderId="24" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="22" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="27" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="37" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="2" fillId="4" borderId="44" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="2" fillId="4" borderId="23" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="29" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="30" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="31" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="32" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="2" fillId="4" borderId="25" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="2" fillId="5" borderId="43" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="6" borderId="30" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="6" borderId="32" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="6" borderId="30" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="48" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="49" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="50" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="51" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="52" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="2" fillId="6" borderId="32" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="31" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="32" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="6" borderId="39" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="6" borderId="41" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1211,7 +1218,147 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="45" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="31" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="32" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="45" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="37" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="25" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="23" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="30" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="32" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="43" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="46" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="47" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="37" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="39" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="45" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="37" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="43" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="46" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="47" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="34" xfId="3" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="49" xfId="3" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="35" xfId="3" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="26" xfId="3" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="50" xfId="3" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="51" xfId="3" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="39" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="39" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="42" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="52" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="47" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="43" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="46" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="47" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="53" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="54" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="55" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="43" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="46" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1220,80 +1367,119 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="47" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="32" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="31" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="4" borderId="24" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="22" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="39" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="27" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="40" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="22" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="4" borderId="54" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="2" fillId="4" borderId="23" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="29" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="6" borderId="30" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="6" borderId="32" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="2" fillId="6" borderId="30" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="6" borderId="32" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="32" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="31" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="30" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="31" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="32" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="2" fillId="4" borderId="25" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="2" fillId="5" borderId="55" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="2" fillId="5" borderId="53" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="5" borderId="42" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="6" borderId="42" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="6" borderId="44" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
     <cellStyle name="40% - Énfasis3" xfId="3" builtinId="39"/>
     <cellStyle name="60% - Énfasis1" xfId="1" builtinId="32"/>
+    <cellStyle name="Millares" xfId="4" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Porcentaje" xfId="2" builtinId="5"/>
   </cellStyles>
-  <dxfs count="11">
+  <dxfs count="13">
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -1339,14 +1525,42 @@
       </font>
       <alignment textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
+        <left style="medium">
           <color indexed="64"/>
         </left>
-        <right style="thin">
+        <right style="medium">
           <color indexed="64"/>
         </right>
         <top/>
         <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -1392,92 +1606,16 @@
       </font>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
+        <left style="medium">
           <color indexed="64"/>
         </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-      <alignment textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
+        <right style="medium">
           <color indexed="64"/>
         </right>
         <top/>
         <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-      <alignment textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-      <alignment textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -1611,17 +1749,19 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{E057D4CC-3DD2-4D81-86A9-18DDFAD09B90}" name="Tabla4" displayName="Tabla4" ref="B18:J19" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9" dataCellStyle="60% - Énfasis1">
-  <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{98B8256F-E26F-4205-A6A8-333E7EAE0F41}" name="N°" dataDxfId="8" dataCellStyle="60% - Énfasis1"/>
-    <tableColumn id="3" xr3:uid="{A0BE3634-DE46-413B-90E6-4196954DEAAA}" name="Descripción" dataDxfId="7" dataCellStyle="60% - Énfasis1"/>
-    <tableColumn id="4" xr3:uid="{63F9F091-914E-4C1D-B3AD-57466FD91CA4}" name="Peso En El Proyecto" dataDxfId="6" dataCellStyle="60% - Énfasis1"/>
-    <tableColumn id="5" xr3:uid="{B0F9A695-0332-403A-B9D5-CB97EBA3F077}" name="Fiabilidad" dataDxfId="5" dataCellStyle="60% - Énfasis1"/>
-    <tableColumn id="6" xr3:uid="{F8C3C4A4-9D62-4CA8-89B4-104417FF70AC}" name="Facilidad De Entendimiento" dataDxfId="4" dataCellStyle="60% - Énfasis1"/>
-    <tableColumn id="2" xr3:uid="{33E5E045-DC9B-49BB-BE97-54FEB20DF2ED}" name="Probabilidad De Modificación" dataDxfId="3" dataCellStyle="60% - Énfasis1"/>
-    <tableColumn id="7" xr3:uid="{9311DDE0-F38A-48A0-A210-585C483D4C54}" name="Calidad" dataDxfId="2" dataCellStyle="60% - Énfasis1"/>
-    <tableColumn id="9" xr3:uid="{73FC66C9-4756-4C2C-A212-4A3AE69350A6}" name="Cumplimiento Entregable" dataDxfId="0" dataCellStyle="60% - Énfasis1"/>
-    <tableColumn id="8" xr3:uid="{FC406A40-64E2-4699-89C6-6293E114A363}" name="Porcentaje De Cumplimiento" dataDxfId="1" dataCellStyle="60% - Énfasis1"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{E057D4CC-3DD2-4D81-86A9-18DDFAD09B90}" name="Tabla4" displayName="Tabla4" ref="B18:L19" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11" dataCellStyle="60% - Énfasis1">
+  <tableColumns count="11">
+    <tableColumn id="1" xr3:uid="{98B8256F-E26F-4205-A6A8-333E7EAE0F41}" name="N°" dataDxfId="10" dataCellStyle="60% - Énfasis1"/>
+    <tableColumn id="3" xr3:uid="{A0BE3634-DE46-413B-90E6-4196954DEAAA}" name="Descripción" dataDxfId="9" dataCellStyle="60% - Énfasis1"/>
+    <tableColumn id="4" xr3:uid="{63F9F091-914E-4C1D-B3AD-57466FD91CA4}" name="Peso En El Proyecto" dataDxfId="1" dataCellStyle="60% - Énfasis1"/>
+    <tableColumn id="5" xr3:uid="{B0F9A695-0332-403A-B9D5-CB97EBA3F077}" name="Fiabilidad" dataDxfId="2" dataCellStyle="60% - Énfasis1"/>
+    <tableColumn id="6" xr3:uid="{F8C3C4A4-9D62-4CA8-89B4-104417FF70AC}" name="Facilidad De Entendimiento" dataDxfId="3" dataCellStyle="60% - Énfasis1"/>
+    <tableColumn id="2" xr3:uid="{33E5E045-DC9B-49BB-BE97-54FEB20DF2ED}" name="Probabilidad De Modificación" dataDxfId="4" dataCellStyle="60% - Énfasis1"/>
+    <tableColumn id="7" xr3:uid="{9311DDE0-F38A-48A0-A210-585C483D4C54}" name="Calidad" dataDxfId="5" dataCellStyle="60% - Énfasis1"/>
+    <tableColumn id="9" xr3:uid="{73FC66C9-4756-4C2C-A212-4A3AE69350A6}" name="Cumplimiento Entregable" dataDxfId="8" dataCellStyle="60% - Énfasis1"/>
+    <tableColumn id="8" xr3:uid="{FC406A40-64E2-4699-89C6-6293E114A363}" name="Porcentaje De Cumplimiento" dataDxfId="6" dataCellStyle="60% - Énfasis1"/>
+    <tableColumn id="10" xr3:uid="{31E184EA-A517-4E3B-894A-67C0DB44E6A6}" name="Pocentaje Por Fase" dataDxfId="7" dataCellStyle="60% - Énfasis1"/>
+    <tableColumn id="11" xr3:uid="{31269059-FB15-4322-8D0A-3E4A875C60EF}" name="Peso Fase" dataDxfId="0" dataCellStyle="60% - Énfasis1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1924,10 +2064,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7014F898-5058-4D1B-9637-B21A5C3439BD}">
-  <dimension ref="A1:J1048570"/>
+  <dimension ref="A1:M1048570"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C52" workbookViewId="0">
-      <selection activeCell="L64" sqref="L64"/>
+    <sheetView tabSelected="1" topLeftCell="D33" workbookViewId="0">
+      <selection activeCell="H39" sqref="H39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1950,7 +2090,7 @@
         <v>73</v>
       </c>
       <c r="F2" s="6"/>
-      <c r="G2" s="20"/>
+      <c r="G2" s="14"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B3" s="72"/>
@@ -1958,7 +2098,7 @@
       <c r="D3" s="74"/>
       <c r="E3" s="75"/>
       <c r="F3" s="76"/>
-      <c r="G3" s="38"/>
+      <c r="G3" s="27"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B4" s="7" t="s">
@@ -1970,7 +2110,7 @@
       <c r="D4" s="77"/>
       <c r="E4" s="78"/>
       <c r="F4" s="79"/>
-      <c r="G4" s="38"/>
+      <c r="G4" s="27"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B5" s="7" t="s">
@@ -1982,10 +2122,10 @@
       <c r="D5" s="77"/>
       <c r="E5" s="78"/>
       <c r="F5" s="79"/>
-      <c r="G5" s="38"/>
+      <c r="G5" s="27"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B6" s="34" t="s">
+      <c r="B6" s="23" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="8">
@@ -1994,7 +2134,7 @@
       <c r="D6" s="77"/>
       <c r="E6" s="78"/>
       <c r="F6" s="79"/>
-      <c r="G6" s="38"/>
+      <c r="G6" s="27"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B7" s="7" t="s">
@@ -2006,7 +2146,7 @@
       <c r="D7" s="77"/>
       <c r="E7" s="78"/>
       <c r="F7" s="79"/>
-      <c r="G7" s="38"/>
+      <c r="G7" s="27"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B8" s="7" t="s">
@@ -2018,10 +2158,10 @@
       <c r="D8" s="77"/>
       <c r="E8" s="78"/>
       <c r="F8" s="79"/>
-      <c r="G8" s="38"/>
+      <c r="G8" s="27"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B9" s="34" t="s">
+      <c r="B9" s="23" t="s">
         <v>7</v>
       </c>
       <c r="C9" s="9">
@@ -2030,7 +2170,7 @@
       <c r="D9" s="77"/>
       <c r="E9" s="78"/>
       <c r="F9" s="79"/>
-      <c r="G9" s="38"/>
+      <c r="G9" s="27"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B10" s="7" t="s">
@@ -2042,7 +2182,7 @@
       <c r="D10" s="80"/>
       <c r="E10" s="81"/>
       <c r="F10" s="82"/>
-      <c r="G10" s="38"/>
+      <c r="G10" s="27"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B11" s="7" t="s">
@@ -2054,7 +2194,7 @@
       <c r="D11" s="84"/>
       <c r="E11" s="84"/>
       <c r="F11" s="85"/>
-      <c r="G11" s="38"/>
+      <c r="G11" s="27"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B12" s="7" t="s">
@@ -2066,1714 +2206,1895 @@
       <c r="D12" s="84"/>
       <c r="E12" s="84"/>
       <c r="F12" s="85"/>
-      <c r="G12" s="38"/>
+      <c r="G12" s="27"/>
     </row>
     <row r="13" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="33" t="s">
+      <c r="B13" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="69" t="s">
+      <c r="C13" s="88" t="s">
         <v>15</v>
       </c>
-      <c r="D13" s="70"/>
-      <c r="E13" s="70"/>
-      <c r="F13" s="71"/>
-      <c r="G13" s="38"/>
+      <c r="D13" s="89"/>
+      <c r="E13" s="89"/>
+      <c r="F13" s="90"/>
+      <c r="G13" s="27"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="20"/>
+      <c r="A15" s="14"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
     </row>
-    <row r="17" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D17" s="63" t="s">
+    <row r="17" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D17" s="87" t="s">
         <v>62</v>
       </c>
-      <c r="E17" s="63"/>
-      <c r="F17" s="63"/>
-      <c r="G17" s="63"/>
-      <c r="H17" s="63"/>
-      <c r="I17" s="63"/>
-      <c r="J17" s="63"/>
-    </row>
-    <row r="18" spans="2:10" ht="30" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="48" t="s">
+      <c r="E17" s="87"/>
+      <c r="F17" s="87"/>
+      <c r="G17" s="87"/>
+      <c r="H17" s="87"/>
+      <c r="I17" s="87"/>
+      <c r="J17" s="87"/>
+      <c r="K17" s="94"/>
+      <c r="L17" s="94"/>
+    </row>
+    <row r="18" spans="2:13" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="37" t="s">
         <v>61</v>
       </c>
-      <c r="C18" s="49" t="s">
+      <c r="C18" s="38" t="s">
         <v>17</v>
       </c>
-      <c r="D18" s="49" t="s">
+      <c r="D18" s="38" t="s">
         <v>63</v>
       </c>
-      <c r="E18" s="62" t="s">
+      <c r="E18" s="48" t="s">
         <v>66</v>
       </c>
-      <c r="F18" s="50" t="s">
+      <c r="F18" s="39" t="s">
         <v>67</v>
       </c>
-      <c r="G18" s="50" t="s">
+      <c r="G18" s="39" t="s">
         <v>68</v>
       </c>
-      <c r="H18" s="61" t="s">
+      <c r="H18" s="47" t="s">
         <v>65</v>
       </c>
-      <c r="I18" s="91" t="s">
+      <c r="I18" s="50" t="s">
         <v>75</v>
       </c>
-      <c r="J18" s="90" t="s">
+      <c r="J18" s="49" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="19" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="10"/>
-      <c r="C19" s="12" t="s">
+      <c r="K18" s="95" t="s">
+        <v>78</v>
+      </c>
+      <c r="L18" s="95" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="19" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="138"/>
+      <c r="C19" s="103" t="s">
         <v>18</v>
       </c>
-      <c r="D19" s="13"/>
-      <c r="E19" s="11"/>
-      <c r="F19" s="11"/>
-      <c r="G19" s="11"/>
-      <c r="H19" s="14"/>
-      <c r="I19" s="98"/>
-      <c r="J19" s="96"/>
-    </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B20" s="87">
+      <c r="D19" s="54"/>
+      <c r="E19" s="54"/>
+      <c r="F19" s="54"/>
+      <c r="G19" s="54"/>
+      <c r="H19" s="54"/>
+      <c r="I19" s="54"/>
+      <c r="J19" s="54"/>
+      <c r="K19" s="106"/>
+      <c r="L19" s="54"/>
+    </row>
+    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B20" s="147">
         <v>1</v>
       </c>
-      <c r="C20" s="15" t="s">
+      <c r="C20" s="134" t="s">
         <v>19</v>
       </c>
-      <c r="D20" s="17">
+      <c r="D20" s="12">
         <v>0.05</v>
       </c>
-      <c r="E20" s="16">
+      <c r="E20" s="11">
         <v>0.05</v>
       </c>
-      <c r="F20" s="16">
+      <c r="F20" s="11">
         <v>0.01</v>
       </c>
-      <c r="G20" s="16">
+      <c r="G20" s="11">
         <v>0.01</v>
       </c>
-      <c r="H20" s="94">
+      <c r="H20" s="51">
         <v>0.05</v>
       </c>
-      <c r="I20" s="97">
+      <c r="I20" s="53">
         <v>1</v>
       </c>
-      <c r="J20" s="99">
+      <c r="J20" s="115">
         <f>D20*I20</f>
         <v>0.05</v>
       </c>
-    </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B21" s="87"/>
-      <c r="C21" s="18" t="s">
+      <c r="K20" s="116">
+        <v>15</v>
+      </c>
+      <c r="L20" s="127">
+        <f>H31*K20/100</f>
+        <v>14.7</v>
+      </c>
+    </row>
+    <row r="21" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B21" s="148"/>
+      <c r="C21" s="131" t="s">
         <v>20</v>
       </c>
-      <c r="D21" s="17">
-        <v>0.1</v>
-      </c>
-      <c r="E21" s="16">
+      <c r="D21" s="12">
+        <v>0.1</v>
+      </c>
+      <c r="E21" s="11">
         <v>0.05</v>
       </c>
-      <c r="F21" s="16">
-        <v>0.1</v>
-      </c>
-      <c r="G21" s="16">
+      <c r="F21" s="11">
+        <v>0.1</v>
+      </c>
+      <c r="G21" s="11">
         <v>0.05</v>
       </c>
-      <c r="H21" s="94">
+      <c r="H21" s="51">
         <v>0.05</v>
       </c>
-      <c r="I21" s="97">
+      <c r="I21" s="53">
         <v>1</v>
       </c>
-      <c r="J21" s="99">
+      <c r="J21" s="111">
         <f t="shared" ref="J21:J30" si="0">D21*I21</f>
         <v>0.1</v>
       </c>
-    </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B22" s="87"/>
-      <c r="C22" s="18" t="s">
+      <c r="K21" s="117"/>
+      <c r="L21" s="128"/>
+    </row>
+    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B22" s="148"/>
+      <c r="C22" s="131" t="s">
         <v>21</v>
       </c>
-      <c r="D22" s="17">
-        <v>0.1</v>
-      </c>
-      <c r="E22" s="16">
-        <v>0.1</v>
-      </c>
-      <c r="F22" s="16">
-        <v>0.1</v>
-      </c>
-      <c r="G22" s="16">
+      <c r="D22" s="12">
+        <v>0.1</v>
+      </c>
+      <c r="E22" s="11">
+        <v>0.1</v>
+      </c>
+      <c r="F22" s="11">
+        <v>0.1</v>
+      </c>
+      <c r="G22" s="11">
         <v>0.05</v>
       </c>
-      <c r="H22" s="94">
+      <c r="H22" s="51">
         <v>0.05</v>
       </c>
-      <c r="I22" s="97">
+      <c r="I22" s="53">
         <v>1</v>
       </c>
-      <c r="J22" s="99">
+      <c r="J22" s="111">
         <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
-    </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B23" s="87"/>
-      <c r="C23" s="18" t="s">
+      <c r="K22" s="117"/>
+      <c r="L22" s="128"/>
+    </row>
+    <row r="23" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B23" s="148"/>
+      <c r="C23" s="131" t="s">
         <v>22</v>
       </c>
-      <c r="D23" s="17">
+      <c r="D23" s="12">
         <v>0.02</v>
       </c>
-      <c r="E23" s="16">
+      <c r="E23" s="11">
         <v>0.05</v>
       </c>
-      <c r="F23" s="16">
+      <c r="F23" s="11">
         <v>0.01</v>
       </c>
-      <c r="G23" s="16">
+      <c r="G23" s="11">
         <v>0.05</v>
       </c>
-      <c r="H23" s="94">
+      <c r="H23" s="51">
         <v>0.02</v>
       </c>
-      <c r="I23" s="97">
+      <c r="I23" s="53">
         <v>1</v>
       </c>
-      <c r="J23" s="99">
+      <c r="J23" s="111">
         <f t="shared" si="0"/>
         <v>0.02</v>
       </c>
-    </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B24" s="88"/>
-      <c r="C24" s="18" t="s">
+      <c r="K23" s="117"/>
+      <c r="L23" s="128"/>
+    </row>
+    <row r="24" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="149"/>
+      <c r="C24" s="131" t="s">
         <v>23</v>
       </c>
-      <c r="D24" s="17">
+      <c r="D24" s="12">
         <v>0.02</v>
       </c>
-      <c r="E24" s="16">
+      <c r="E24" s="11">
         <v>0.05</v>
       </c>
-      <c r="F24" s="16">
+      <c r="F24" s="11">
         <v>0.01</v>
       </c>
-      <c r="G24" s="16">
+      <c r="G24" s="11">
         <v>0.33</v>
       </c>
-      <c r="H24" s="94">
+      <c r="H24" s="51">
         <v>0.02</v>
       </c>
-      <c r="I24" s="97">
+      <c r="I24" s="53">
         <v>1</v>
       </c>
-      <c r="J24" s="99">
+      <c r="J24" s="111">
         <f t="shared" si="0"/>
         <v>0.02</v>
       </c>
-    </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B25" s="89">
+      <c r="K24" s="117"/>
+      <c r="L24" s="128"/>
+    </row>
+    <row r="25" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B25" s="147">
         <v>2</v>
       </c>
-      <c r="C25" s="18" t="s">
+      <c r="C25" s="131" t="s">
         <v>24</v>
       </c>
-      <c r="D25" s="17">
-        <v>0.1</v>
-      </c>
-      <c r="E25" s="17">
-        <v>0.1</v>
-      </c>
-      <c r="F25" s="16">
+      <c r="D25" s="12">
+        <v>0.1</v>
+      </c>
+      <c r="E25" s="12">
+        <v>0.1</v>
+      </c>
+      <c r="F25" s="11">
         <v>0.05</v>
       </c>
-      <c r="G25" s="16">
+      <c r="G25" s="11">
         <v>0.01</v>
       </c>
-      <c r="H25" s="94">
-        <v>0.2</v>
-      </c>
-      <c r="I25" s="97">
+      <c r="H25" s="51">
+        <v>0.2</v>
+      </c>
+      <c r="I25" s="53">
         <v>1</v>
       </c>
-      <c r="J25" s="99">
+      <c r="J25" s="111">
         <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
-    </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B26" s="87"/>
-      <c r="C26" s="18" t="s">
+      <c r="K25" s="117"/>
+      <c r="L25" s="128"/>
+    </row>
+    <row r="26" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B26" s="148"/>
+      <c r="C26" s="131" t="s">
         <v>25</v>
       </c>
-      <c r="D26" s="17">
-        <v>0.1</v>
-      </c>
-      <c r="E26" s="17">
-        <v>0.1</v>
-      </c>
-      <c r="F26" s="16">
-        <v>0.1</v>
-      </c>
-      <c r="G26" s="16">
+      <c r="D26" s="12">
+        <v>0.1</v>
+      </c>
+      <c r="E26" s="12">
+        <v>0.1</v>
+      </c>
+      <c r="F26" s="11">
+        <v>0.1</v>
+      </c>
+      <c r="G26" s="11">
         <v>0.05</v>
       </c>
-      <c r="H26" s="94">
+      <c r="H26" s="51">
         <v>0.05</v>
       </c>
-      <c r="I26" s="97">
+      <c r="I26" s="53">
         <v>1</v>
       </c>
-      <c r="J26" s="99">
+      <c r="J26" s="111">
         <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
-    </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B27" s="87"/>
-      <c r="C27" s="18" t="s">
+      <c r="K26" s="117"/>
+      <c r="L26" s="128"/>
+    </row>
+    <row r="27" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B27" s="148"/>
+      <c r="C27" s="131" t="s">
         <v>26</v>
       </c>
-      <c r="D27" s="17">
+      <c r="D27" s="12">
+        <v>0.2</v>
+      </c>
+      <c r="E27" s="12">
         <v>0.15</v>
       </c>
-      <c r="E27" s="17">
+      <c r="F27" s="11">
         <v>0.15</v>
       </c>
-      <c r="F27" s="16">
+      <c r="G27" s="11">
+        <v>0.05</v>
+      </c>
+      <c r="H27" s="51">
+        <v>0.1</v>
+      </c>
+      <c r="I27" s="53">
+        <v>1</v>
+      </c>
+      <c r="J27" s="111">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
+      <c r="K27" s="117"/>
+      <c r="L27" s="128"/>
+      <c r="M27" s="105"/>
+    </row>
+    <row r="28" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B28" s="148"/>
+      <c r="C28" s="131" t="s">
+        <v>27</v>
+      </c>
+      <c r="D28" s="12">
+        <v>0.06</v>
+      </c>
+      <c r="E28" s="12">
         <v>0.15</v>
       </c>
-      <c r="G27" s="16">
+      <c r="F28" s="11">
+        <v>0.2</v>
+      </c>
+      <c r="G28" s="11">
         <v>0.05</v>
       </c>
-      <c r="H27" s="94">
-        <v>0.1</v>
-      </c>
-      <c r="I27" s="97">
+      <c r="H28" s="51">
+        <v>0.26</v>
+      </c>
+      <c r="I28" s="53">
         <v>1</v>
       </c>
-      <c r="J27" s="99">
+      <c r="J28" s="111">
         <f t="shared" si="0"/>
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B28" s="87"/>
-      <c r="C28" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="D28" s="17">
-        <v>0.1</v>
-      </c>
-      <c r="E28" s="17">
-        <v>0.15</v>
-      </c>
-      <c r="F28" s="16">
-        <v>0.2</v>
-      </c>
-      <c r="G28" s="16">
+        <v>0.06</v>
+      </c>
+      <c r="K28" s="117"/>
+      <c r="L28" s="128"/>
+    </row>
+    <row r="29" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B29" s="148"/>
+      <c r="C29" s="131" t="s">
+        <v>28</v>
+      </c>
+      <c r="D29" s="12">
+        <v>0.1</v>
+      </c>
+      <c r="E29" s="12">
+        <v>0.1</v>
+      </c>
+      <c r="F29" s="11">
+        <v>0.1</v>
+      </c>
+      <c r="G29" s="11">
         <v>0.05</v>
       </c>
-      <c r="H28" s="94">
-        <v>0.26</v>
-      </c>
-      <c r="I28" s="97">
+      <c r="H29" s="51">
+        <v>0.1</v>
+      </c>
+      <c r="I29" s="53">
         <v>1</v>
       </c>
-      <c r="J28" s="99">
+      <c r="J29" s="111">
         <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
-    </row>
-    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B29" s="87"/>
-      <c r="C29" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="D29" s="17">
-        <v>0.1</v>
-      </c>
-      <c r="E29" s="17">
-        <v>0.1</v>
-      </c>
-      <c r="F29" s="16">
-        <v>0.1</v>
-      </c>
-      <c r="G29" s="16">
+      <c r="K29" s="117"/>
+      <c r="L29" s="128"/>
+    </row>
+    <row r="30" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="149"/>
+      <c r="C30" s="131" t="s">
+        <v>29</v>
+      </c>
+      <c r="D30" s="12">
+        <v>0.11</v>
+      </c>
+      <c r="E30" s="12">
         <v>0.05</v>
       </c>
-      <c r="H29" s="94">
-        <v>0.1</v>
-      </c>
-      <c r="I29" s="97">
-        <v>1</v>
-      </c>
-      <c r="J29" s="99">
+      <c r="F30" s="11">
+        <v>0.12</v>
+      </c>
+      <c r="G30" s="11">
+        <v>0.2</v>
+      </c>
+      <c r="H30" s="51">
+        <v>0.05</v>
+      </c>
+      <c r="I30" s="57">
+        <v>0.98</v>
+      </c>
+      <c r="J30" s="112">
         <f t="shared" si="0"/>
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="30" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="87"/>
-      <c r="C30" s="18" t="s">
-        <v>29</v>
-      </c>
-      <c r="D30" s="17">
-        <v>0.11</v>
-      </c>
-      <c r="E30" s="17">
-        <v>0.05</v>
-      </c>
-      <c r="F30" s="16">
-        <v>0.12</v>
-      </c>
-      <c r="G30" s="16">
-        <v>0.2</v>
-      </c>
-      <c r="H30" s="94">
-        <v>0.05</v>
-      </c>
-      <c r="I30" s="102">
-        <v>1</v>
-      </c>
-      <c r="J30" s="103">
-        <f t="shared" si="0"/>
-        <v>0.11</v>
-      </c>
-    </row>
-    <row r="31" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="56" t="s">
+        <v>0.10779999999999999</v>
+      </c>
+      <c r="K30" s="118"/>
+      <c r="L30" s="129"/>
+    </row>
+    <row r="31" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="140" t="s">
         <v>64</v>
       </c>
-      <c r="C31" s="57"/>
-      <c r="D31" s="59">
+      <c r="C31" s="43"/>
+      <c r="D31" s="45">
         <f>SUM(D20:D30)</f>
-        <v>0.95</v>
-      </c>
-      <c r="E31" s="59">
+        <v>0.96</v>
+      </c>
+      <c r="E31" s="45">
         <f>SUM(E20:E30)</f>
         <v>0.95000000000000007</v>
       </c>
-      <c r="F31" s="60">
+      <c r="F31" s="46">
         <f>SUM(F20:F30)</f>
         <v>0.95</v>
       </c>
-      <c r="G31" s="60">
+      <c r="G31" s="46">
         <f>SUM(G20:G30)</f>
         <v>0.90000000000000013</v>
       </c>
-      <c r="H31" s="60">
-        <f>SUM(H20:H30)</f>
-        <v>0.95000000000000007</v>
-      </c>
-      <c r="I31" s="104">
-        <f>SUM(J20:J30)</f>
-        <v>0.95</v>
-      </c>
-      <c r="J31" s="105"/>
-    </row>
-    <row r="32" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="23"/>
-      <c r="C32" s="25" t="s">
+      <c r="H31" s="104">
+        <v>98</v>
+      </c>
+      <c r="I31" s="113">
+        <v>96</v>
+      </c>
+      <c r="J31" s="114"/>
+      <c r="K31" s="109" t="s">
+        <v>77</v>
+      </c>
+      <c r="L31" s="107"/>
+    </row>
+    <row r="32" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="137"/>
+      <c r="C32" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="D32" s="24"/>
-      <c r="E32" s="24"/>
-      <c r="F32" s="93"/>
-      <c r="G32" s="93"/>
-      <c r="H32" s="93"/>
-      <c r="I32" s="93"/>
+      <c r="D32" s="16"/>
+      <c r="E32" s="16"/>
+      <c r="F32" s="91"/>
+      <c r="G32" s="91"/>
+      <c r="H32" s="91"/>
+      <c r="I32" s="91"/>
       <c r="J32" s="92"/>
-    </row>
-    <row r="33" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B33" s="64">
+      <c r="K32" s="110"/>
+      <c r="L32" s="108"/>
+    </row>
+    <row r="33" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B33" s="144">
         <v>3</v>
       </c>
-      <c r="C33" s="15" t="s">
+      <c r="C33" s="134" t="s">
         <v>31</v>
       </c>
-      <c r="D33" s="17">
+      <c r="D33" s="12">
         <v>0.05</v>
       </c>
-      <c r="E33" s="43" t="s">
+      <c r="E33" s="32" t="s">
         <v>69</v>
       </c>
-      <c r="F33" s="46" t="s">
+      <c r="F33" s="35" t="s">
         <v>69</v>
       </c>
-      <c r="G33" s="47" t="s">
+      <c r="G33" s="36" t="s">
         <v>69</v>
       </c>
-      <c r="H33" s="100">
-        <v>0.1</v>
-      </c>
-      <c r="I33" s="97">
+      <c r="H33" s="55">
+        <v>0.1</v>
+      </c>
+      <c r="I33" s="53">
         <v>1</v>
       </c>
-      <c r="J33" s="106">
+      <c r="J33" s="101">
         <f>D33*I33</f>
         <v>0.05</v>
       </c>
-    </row>
-    <row r="34" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B34" s="65"/>
-      <c r="C34" s="18" t="s">
+      <c r="K33" s="116">
+        <v>15</v>
+      </c>
+      <c r="L33" s="98">
+        <f>H39*K33/100</f>
+        <v>14.7</v>
+      </c>
+    </row>
+    <row r="34" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B34" s="145"/>
+      <c r="C34" s="131" t="s">
         <v>32</v>
       </c>
-      <c r="D34" s="17">
+      <c r="D34" s="12">
         <v>0.25</v>
       </c>
-      <c r="E34" s="17">
+      <c r="E34" s="12">
         <v>0.35</v>
       </c>
-      <c r="F34" s="26">
+      <c r="F34" s="18">
         <v>0.25</v>
       </c>
-      <c r="G34" s="39">
+      <c r="G34" s="28">
         <v>0.45</v>
       </c>
-      <c r="H34" s="101">
+      <c r="H34" s="56">
         <v>0.25</v>
       </c>
-      <c r="I34" s="95">
+      <c r="I34" s="52">
         <v>0.98</v>
       </c>
-      <c r="J34" s="106">
+      <c r="J34" s="101">
         <f t="shared" ref="J34:J38" si="1">D34*I34</f>
         <v>0.245</v>
       </c>
-    </row>
-    <row r="35" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B35" s="65"/>
-      <c r="C35" s="18" t="s">
+      <c r="K34" s="117"/>
+      <c r="L34" s="99"/>
+    </row>
+    <row r="35" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B35" s="145"/>
+      <c r="C35" s="131" t="s">
         <v>37</v>
       </c>
-      <c r="D35" s="17">
-        <v>0.2</v>
-      </c>
-      <c r="E35" s="17">
-        <v>0.2</v>
-      </c>
-      <c r="F35" s="26">
+      <c r="D35" s="12">
+        <v>0.2</v>
+      </c>
+      <c r="E35" s="12">
+        <v>0.2</v>
+      </c>
+      <c r="F35" s="18">
         <v>0.3</v>
       </c>
-      <c r="G35" s="39">
-        <v>0.2</v>
-      </c>
-      <c r="H35" s="101">
+      <c r="G35" s="28">
+        <v>0.2</v>
+      </c>
+      <c r="H35" s="56">
         <v>0.3</v>
       </c>
-      <c r="I35" s="95">
+      <c r="I35" s="52">
         <v>0.98</v>
       </c>
-      <c r="J35" s="106">
+      <c r="J35" s="101">
         <f t="shared" si="1"/>
         <v>0.19600000000000001</v>
       </c>
-    </row>
-    <row r="36" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B36" s="65"/>
-      <c r="C36" s="18" t="s">
+      <c r="K35" s="117"/>
+      <c r="L35" s="99"/>
+    </row>
+    <row r="36" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B36" s="145"/>
+      <c r="C36" s="131" t="s">
         <v>33</v>
       </c>
-      <c r="D36" s="17">
+      <c r="D36" s="12">
         <v>0.01</v>
       </c>
-      <c r="E36" s="43" t="s">
+      <c r="E36" s="32" t="s">
         <v>69</v>
       </c>
-      <c r="F36" s="44" t="s">
+      <c r="F36" s="33" t="s">
         <v>69</v>
       </c>
-      <c r="G36" s="45" t="s">
+      <c r="G36" s="34" t="s">
         <v>70</v>
       </c>
-      <c r="H36" s="101">
+      <c r="H36" s="56">
         <v>0.01</v>
       </c>
-      <c r="I36" s="95">
+      <c r="I36" s="52">
         <v>0.98</v>
       </c>
-      <c r="J36" s="106">
+      <c r="J36" s="101">
         <f t="shared" si="1"/>
         <v>9.7999999999999997E-3</v>
       </c>
-    </row>
-    <row r="37" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B37" s="65"/>
-      <c r="C37" s="18" t="s">
+      <c r="K36" s="117"/>
+      <c r="L36" s="99"/>
+    </row>
+    <row r="37" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B37" s="145"/>
+      <c r="C37" s="131" t="s">
         <v>34</v>
       </c>
-      <c r="D37" s="17">
+      <c r="D37" s="12">
         <v>0.14000000000000001</v>
       </c>
-      <c r="E37" s="17">
-        <v>0.1</v>
-      </c>
-      <c r="F37" s="26">
-        <v>0.2</v>
-      </c>
-      <c r="G37" s="39">
-        <v>0.1</v>
-      </c>
-      <c r="H37" s="101">
-        <v>0.2</v>
-      </c>
-      <c r="I37" s="95">
+      <c r="E37" s="12">
+        <v>0.1</v>
+      </c>
+      <c r="F37" s="18">
+        <v>0.2</v>
+      </c>
+      <c r="G37" s="28">
+        <v>0.1</v>
+      </c>
+      <c r="H37" s="56">
+        <v>0.2</v>
+      </c>
+      <c r="I37" s="52">
         <v>1</v>
       </c>
-      <c r="J37" s="106">
+      <c r="J37" s="101">
         <f t="shared" si="1"/>
         <v>0.14000000000000001</v>
       </c>
-    </row>
-    <row r="38" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="66"/>
-      <c r="C38" s="21" t="s">
+      <c r="K37" s="117"/>
+      <c r="L37" s="99"/>
+    </row>
+    <row r="38" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B38" s="146"/>
+      <c r="C38" s="135" t="s">
         <v>35</v>
       </c>
-      <c r="D38" s="37">
+      <c r="D38" s="26">
+        <v>0.33</v>
+      </c>
+      <c r="E38" s="26">
         <v>0.3</v>
       </c>
-      <c r="E38" s="37">
-        <v>0.3</v>
-      </c>
-      <c r="F38" s="39">
-        <v>0.2</v>
-      </c>
-      <c r="G38" s="39">
-        <v>0.2</v>
-      </c>
-      <c r="H38" s="101">
+      <c r="F38" s="28">
+        <v>0.2</v>
+      </c>
+      <c r="G38" s="28">
+        <v>0.2</v>
+      </c>
+      <c r="H38" s="56">
         <v>0.09</v>
       </c>
-      <c r="I38" s="107">
-        <v>0.9</v>
-      </c>
-      <c r="J38" s="108">
+      <c r="I38" s="58">
+        <v>0.95</v>
+      </c>
+      <c r="J38" s="102">
         <f t="shared" si="1"/>
-        <v>0.27</v>
-      </c>
-    </row>
-    <row r="39" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="56" t="s">
+        <v>0.3135</v>
+      </c>
+      <c r="K38" s="118"/>
+      <c r="L38" s="100"/>
+    </row>
+    <row r="39" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B39" s="140" t="s">
         <v>64</v>
       </c>
-      <c r="C39" s="57"/>
-      <c r="D39" s="58">
+      <c r="C39" s="43"/>
+      <c r="D39" s="44">
         <f>SUM(D33:D38)</f>
-        <v>0.95</v>
-      </c>
-      <c r="E39" s="58">
+        <v>0.98</v>
+      </c>
+      <c r="E39" s="44">
         <f>SUM(E33:E38)</f>
         <v>0.95</v>
       </c>
-      <c r="F39" s="58">
+      <c r="F39" s="44">
         <f>SUM(F33:F38)</f>
         <v>0.95</v>
       </c>
-      <c r="G39" s="58">
+      <c r="G39" s="44">
         <f>SUM(G33:G38)</f>
         <v>0.95</v>
       </c>
-      <c r="H39" s="58">
-        <f>SUM(H33:H38)</f>
-        <v>0.94999999999999984</v>
-      </c>
-      <c r="I39" s="104">
+      <c r="H39" s="122">
+        <v>98</v>
+      </c>
+      <c r="I39" s="66">
         <f>SUM(J33:J38)</f>
-        <v>0.91080000000000005</v>
-      </c>
-      <c r="J39" s="105"/>
-    </row>
-    <row r="40" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="28"/>
-      <c r="C40" s="25" t="s">
+        <v>0.95430000000000004</v>
+      </c>
+      <c r="J39" s="67"/>
+      <c r="K39" s="94"/>
+      <c r="L39" s="107"/>
+    </row>
+    <row r="40" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B40" s="136"/>
+      <c r="C40" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="D40" s="29"/>
-      <c r="E40" s="29"/>
-      <c r="F40" s="112"/>
-      <c r="G40" s="112"/>
-      <c r="H40" s="112"/>
-      <c r="I40" s="112"/>
-      <c r="J40" s="111"/>
-    </row>
-    <row r="41" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B41" s="64">
+      <c r="D40" s="20"/>
+      <c r="E40" s="20"/>
+      <c r="F40" s="68"/>
+      <c r="G40" s="68"/>
+      <c r="H40" s="68"/>
+      <c r="I40" s="68"/>
+      <c r="J40" s="69"/>
+      <c r="K40" s="94"/>
+      <c r="L40" s="108"/>
+    </row>
+    <row r="41" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B41" s="144">
         <v>4</v>
       </c>
-      <c r="C41" s="15" t="s">
+      <c r="C41" s="134" t="s">
         <v>38</v>
       </c>
-      <c r="D41" s="42">
-        <v>0.2</v>
-      </c>
-      <c r="E41" s="42">
-        <v>0.1</v>
-      </c>
-      <c r="F41" s="36">
+      <c r="D41" s="31">
+        <v>0.2</v>
+      </c>
+      <c r="E41" s="31">
+        <v>0.1</v>
+      </c>
+      <c r="F41" s="25">
         <v>0.05</v>
       </c>
-      <c r="G41" s="36">
-        <v>0.1</v>
-      </c>
-      <c r="H41" s="100">
-        <v>0.1</v>
-      </c>
-      <c r="I41" s="97">
+      <c r="G41" s="25">
+        <v>0.1</v>
+      </c>
+      <c r="H41" s="55">
+        <v>0.1</v>
+      </c>
+      <c r="I41" s="53">
         <v>0.98</v>
       </c>
-      <c r="J41" s="116">
+      <c r="J41" s="96">
         <f>D41*I41</f>
         <v>0.19600000000000001</v>
       </c>
-    </row>
-    <row r="42" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B42" s="65"/>
-      <c r="C42" s="18" t="s">
+      <c r="K41" s="119">
+        <v>30</v>
+      </c>
+      <c r="L41" s="98">
+        <f>H46*K41/100</f>
+        <v>28.5</v>
+      </c>
+    </row>
+    <row r="42" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B42" s="145"/>
+      <c r="C42" s="131" t="s">
         <v>39</v>
       </c>
-      <c r="D42" s="41">
+      <c r="D42" s="30">
         <v>0.15</v>
       </c>
-      <c r="E42" s="41">
-        <v>0.2</v>
-      </c>
-      <c r="F42" s="22">
+      <c r="E42" s="30">
+        <v>0.2</v>
+      </c>
+      <c r="F42" s="15">
         <v>0.05</v>
       </c>
-      <c r="G42" s="22">
+      <c r="G42" s="15">
         <v>0.28999999999999998</v>
       </c>
-      <c r="H42" s="101">
-        <v>0.2</v>
-      </c>
-      <c r="I42" s="95">
-        <v>0.97</v>
-      </c>
-      <c r="J42" s="116">
+      <c r="H42" s="56">
+        <v>0.2</v>
+      </c>
+      <c r="I42" s="52">
+        <v>1</v>
+      </c>
+      <c r="J42" s="96">
         <f t="shared" ref="J42:J45" si="2">D42*I42</f>
-        <v>0.14549999999999999</v>
-      </c>
-    </row>
-    <row r="43" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B43" s="65"/>
-      <c r="C43" s="18" t="s">
+        <v>0.15</v>
+      </c>
+      <c r="K42" s="120"/>
+      <c r="L42" s="99"/>
+    </row>
+    <row r="43" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B43" s="145"/>
+      <c r="C43" s="131" t="s">
         <v>40</v>
       </c>
-      <c r="D43" s="41">
-        <v>0.1</v>
-      </c>
-      <c r="E43" s="42">
-        <v>0.1</v>
-      </c>
-      <c r="F43" s="22">
-        <v>0.2</v>
-      </c>
-      <c r="G43" s="22">
-        <v>0.2</v>
-      </c>
-      <c r="H43" s="101">
-        <v>0.1</v>
-      </c>
-      <c r="I43" s="95">
+      <c r="D43" s="30">
+        <v>0.15</v>
+      </c>
+      <c r="E43" s="31">
+        <v>0.1</v>
+      </c>
+      <c r="F43" s="15">
+        <v>0.2</v>
+      </c>
+      <c r="G43" s="15">
+        <v>0.2</v>
+      </c>
+      <c r="H43" s="56">
+        <v>0.1</v>
+      </c>
+      <c r="I43" s="52">
         <v>0.98</v>
       </c>
-      <c r="J43" s="116">
+      <c r="J43" s="96">
         <f t="shared" si="2"/>
-        <v>9.8000000000000004E-2</v>
-      </c>
-    </row>
-    <row r="44" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B44" s="65"/>
-      <c r="C44" s="18" t="s">
+        <v>0.14699999999999999</v>
+      </c>
+      <c r="K43" s="120"/>
+      <c r="L43" s="99"/>
+    </row>
+    <row r="44" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B44" s="145"/>
+      <c r="C44" s="131" t="s">
         <v>41</v>
       </c>
-      <c r="D44" s="41">
+      <c r="D44" s="30">
         <v>0.4</v>
       </c>
-      <c r="E44" s="41">
+      <c r="E44" s="30">
         <v>0.35</v>
       </c>
-      <c r="F44" s="22">
-        <v>0.1</v>
-      </c>
-      <c r="G44" s="22">
+      <c r="F44" s="15">
+        <v>0.1</v>
+      </c>
+      <c r="G44" s="15">
         <v>0.35</v>
       </c>
-      <c r="H44" s="101">
+      <c r="H44" s="56">
         <v>0.45</v>
       </c>
-      <c r="I44" s="95">
-        <v>0.97</v>
-      </c>
-      <c r="J44" s="116">
+      <c r="I44" s="52">
+        <v>1</v>
+      </c>
+      <c r="J44" s="96">
         <f t="shared" si="2"/>
-        <v>0.38800000000000001</v>
-      </c>
-    </row>
-    <row r="45" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="66"/>
-      <c r="C45" s="21" t="s">
+        <v>0.4</v>
+      </c>
+      <c r="K44" s="120"/>
+      <c r="L44" s="99"/>
+    </row>
+    <row r="45" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B45" s="146"/>
+      <c r="C45" s="135" t="s">
         <v>42</v>
       </c>
-      <c r="D45" s="37">
-        <v>0.1</v>
-      </c>
-      <c r="E45" s="37">
-        <v>0.2</v>
-      </c>
-      <c r="F45" s="22">
+      <c r="D45" s="26">
+        <v>0.1</v>
+      </c>
+      <c r="E45" s="26">
+        <v>0.2</v>
+      </c>
+      <c r="F45" s="15">
         <v>0.55000000000000004</v>
       </c>
-      <c r="G45" s="22">
+      <c r="G45" s="15">
         <v>0.01</v>
       </c>
-      <c r="H45" s="101">
-        <v>0.1</v>
-      </c>
-      <c r="I45" s="107">
+      <c r="H45" s="56">
+        <v>0.1</v>
+      </c>
+      <c r="I45" s="58">
         <v>1</v>
       </c>
-      <c r="J45" s="117">
+      <c r="J45" s="97">
         <f t="shared" si="2"/>
         <v>0.1</v>
       </c>
-    </row>
-    <row r="46" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B46" s="56" t="s">
+      <c r="K45" s="121"/>
+      <c r="L45" s="100"/>
+    </row>
+    <row r="46" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B46" s="140" t="s">
         <v>64</v>
       </c>
-      <c r="C46" s="57"/>
-      <c r="D46" s="58">
+      <c r="C46" s="43"/>
+      <c r="D46" s="44">
         <f>SUM(D41:D45)</f>
-        <v>0.95</v>
-      </c>
-      <c r="E46" s="120">
+        <v>1</v>
+      </c>
+      <c r="E46" s="63">
         <f>SUM(E41:E45)</f>
         <v>0.95</v>
       </c>
-      <c r="F46" s="120">
+      <c r="F46" s="63">
         <f>SUM(F41:F45)</f>
         <v>0.95000000000000007</v>
       </c>
-      <c r="G46" s="120">
+      <c r="G46" s="63">
         <f>SUM(G41:G45)</f>
         <v>0.95000000000000007</v>
       </c>
-      <c r="H46" s="121">
-        <f>SUM(H41:H45)</f>
-        <v>0.95000000000000007</v>
-      </c>
-      <c r="I46" s="122">
+      <c r="H46" s="123">
+        <v>95</v>
+      </c>
+      <c r="I46" s="70">
         <f>SUM(J41:J45)</f>
-        <v>0.92749999999999999</v>
-      </c>
-      <c r="J46" s="123"/>
-    </row>
-    <row r="47" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B47" s="28"/>
-      <c r="C47" s="25" t="s">
+        <v>0.99299999999999999</v>
+      </c>
+      <c r="J46" s="71"/>
+      <c r="K46" s="94"/>
+      <c r="L46" s="107"/>
+    </row>
+    <row r="47" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B47" s="136"/>
+      <c r="C47" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="D47" s="112"/>
-      <c r="E47" s="112"/>
-      <c r="F47" s="112"/>
-      <c r="G47" s="112"/>
-      <c r="H47" s="112"/>
-      <c r="I47" s="112"/>
-      <c r="J47" s="111"/>
-    </row>
-    <row r="48" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B48" s="64">
+      <c r="D47" s="68"/>
+      <c r="E47" s="68"/>
+      <c r="F47" s="68"/>
+      <c r="G47" s="68"/>
+      <c r="H47" s="68"/>
+      <c r="I47" s="68"/>
+      <c r="J47" s="69"/>
+      <c r="K47" s="94"/>
+      <c r="L47" s="108"/>
+    </row>
+    <row r="48" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B48" s="144">
         <v>5</v>
       </c>
-      <c r="C48" s="30" t="s">
+      <c r="C48" s="130" t="s">
         <v>44</v>
       </c>
-      <c r="D48" s="40">
-        <v>0.2</v>
-      </c>
-      <c r="E48" s="42">
-        <v>0.2</v>
-      </c>
-      <c r="F48" s="35">
-        <v>0.2</v>
-      </c>
-      <c r="G48" s="35">
+      <c r="D48" s="29">
+        <v>0.2</v>
+      </c>
+      <c r="E48" s="31">
+        <v>0.2</v>
+      </c>
+      <c r="F48" s="24">
+        <v>0.2</v>
+      </c>
+      <c r="G48" s="24">
         <v>0.18</v>
       </c>
-      <c r="H48" s="100">
-        <v>0.1</v>
-      </c>
-      <c r="I48" s="97">
+      <c r="H48" s="55">
+        <v>0.1</v>
+      </c>
+      <c r="I48" s="53">
         <v>0.99</v>
       </c>
-      <c r="J48" s="106">
+      <c r="J48" s="101">
         <f>D48*I48</f>
         <v>0.19800000000000001</v>
       </c>
-    </row>
-    <row r="49" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B49" s="65"/>
-      <c r="C49" s="18" t="s">
+      <c r="K48" s="116">
+        <v>15</v>
+      </c>
+      <c r="L48" s="98">
+        <f>H54*K48/100</f>
+        <v>14.25</v>
+      </c>
+    </row>
+    <row r="49" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B49" s="145"/>
+      <c r="C49" s="131" t="s">
         <v>45</v>
       </c>
-      <c r="D49" s="41">
-        <v>0.1</v>
-      </c>
-      <c r="E49" s="42">
+      <c r="D49" s="30">
+        <v>0.1</v>
+      </c>
+      <c r="E49" s="31">
         <v>0.08</v>
       </c>
-      <c r="F49" s="27">
+      <c r="F49" s="19">
         <v>0.05</v>
       </c>
-      <c r="G49" s="27">
-        <v>0.2</v>
-      </c>
-      <c r="H49" s="101">
-        <v>0.1</v>
-      </c>
-      <c r="I49" s="95">
+      <c r="G49" s="19">
+        <v>0.2</v>
+      </c>
+      <c r="H49" s="56">
+        <v>0.1</v>
+      </c>
+      <c r="I49" s="52">
         <v>0.99</v>
       </c>
-      <c r="J49" s="106">
+      <c r="J49" s="101">
         <f t="shared" ref="J49:J52" si="3">D49*I49</f>
         <v>9.9000000000000005E-2</v>
       </c>
-    </row>
-    <row r="50" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B50" s="65"/>
-      <c r="C50" s="18" t="s">
+      <c r="K49" s="117"/>
+      <c r="L49" s="99"/>
+    </row>
+    <row r="50" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B50" s="145"/>
+      <c r="C50" s="131" t="s">
         <v>46</v>
       </c>
-      <c r="D50" s="41">
+      <c r="D50" s="30">
         <v>0.15</v>
       </c>
-      <c r="E50" s="42">
-        <v>0.2</v>
-      </c>
-      <c r="F50" s="27">
-        <v>0.2</v>
-      </c>
-      <c r="G50" s="27">
-        <v>0.1</v>
-      </c>
-      <c r="H50" s="101">
-        <v>0.1</v>
-      </c>
-      <c r="I50" s="95">
+      <c r="E50" s="31">
+        <v>0.2</v>
+      </c>
+      <c r="F50" s="19">
+        <v>0.2</v>
+      </c>
+      <c r="G50" s="19">
+        <v>0.1</v>
+      </c>
+      <c r="H50" s="56">
+        <v>0.1</v>
+      </c>
+      <c r="I50" s="52">
         <v>1</v>
       </c>
-      <c r="J50" s="106">
+      <c r="J50" s="101">
         <f t="shared" si="3"/>
         <v>0.15</v>
       </c>
-    </row>
-    <row r="51" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B51" s="65"/>
-      <c r="C51" s="18" t="s">
+      <c r="K50" s="117"/>
+      <c r="L50" s="99"/>
+    </row>
+    <row r="51" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B51" s="145"/>
+      <c r="C51" s="131" t="s">
         <v>47</v>
       </c>
-      <c r="D51" s="41">
-        <v>0.48</v>
-      </c>
-      <c r="E51" s="41">
+      <c r="D51" s="30">
+        <v>0.5</v>
+      </c>
+      <c r="E51" s="30">
         <v>0.45</v>
       </c>
-      <c r="F51" s="27">
+      <c r="F51" s="19">
         <v>0.05</v>
       </c>
-      <c r="G51" s="27">
+      <c r="G51" s="19">
         <v>0.45</v>
       </c>
-      <c r="H51" s="101">
+      <c r="H51" s="56">
         <v>0.45</v>
       </c>
-      <c r="I51" s="95">
+      <c r="I51" s="52">
         <v>0.98</v>
       </c>
-      <c r="J51" s="106">
+      <c r="J51" s="101">
         <f t="shared" si="3"/>
-        <v>0.47039999999999998</v>
-      </c>
-    </row>
-    <row r="52" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B52" s="65"/>
-      <c r="C52" s="18" t="s">
+        <v>0.49</v>
+      </c>
+      <c r="K51" s="117"/>
+      <c r="L51" s="99"/>
+    </row>
+    <row r="52" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B52" s="145"/>
+      <c r="C52" s="131" t="s">
         <v>48</v>
       </c>
-      <c r="D52" s="42">
+      <c r="D52" s="31">
         <v>0.01</v>
       </c>
-      <c r="E52" s="42">
+      <c r="E52" s="31">
         <v>0.01</v>
       </c>
-      <c r="F52" s="27">
+      <c r="F52" s="19">
         <v>0.35</v>
       </c>
-      <c r="G52" s="27">
+      <c r="G52" s="19">
         <v>0.01</v>
       </c>
-      <c r="H52" s="101">
-        <v>0.1</v>
-      </c>
-      <c r="I52" s="95">
+      <c r="H52" s="56">
+        <v>0.1</v>
+      </c>
+      <c r="I52" s="52">
         <v>1</v>
       </c>
-      <c r="J52" s="106">
+      <c r="J52" s="101">
         <f t="shared" si="3"/>
         <v>0.01</v>
       </c>
-    </row>
-    <row r="53" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B53" s="66"/>
-      <c r="C53" s="31" t="s">
+      <c r="K52" s="117"/>
+      <c r="L52" s="99"/>
+    </row>
+    <row r="53" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B53" s="146"/>
+      <c r="C53" s="132" t="s">
         <v>49</v>
       </c>
-      <c r="D53" s="37">
+      <c r="D53" s="26">
         <v>0.01</v>
       </c>
-      <c r="E53" s="37">
+      <c r="E53" s="26">
         <v>0.01</v>
       </c>
-      <c r="F53" s="27">
-        <v>0.1</v>
-      </c>
-      <c r="G53" s="27">
+      <c r="F53" s="19">
+        <v>0.1</v>
+      </c>
+      <c r="G53" s="19">
         <v>0.01</v>
       </c>
-      <c r="H53" s="101">
-        <v>0.1</v>
-      </c>
-      <c r="I53" s="107">
+      <c r="H53" s="56">
+        <v>0.1</v>
+      </c>
+      <c r="I53" s="58">
         <v>1</v>
       </c>
-      <c r="J53" s="106">
+      <c r="J53" s="101">
         <f>D53*I53</f>
         <v>0.01</v>
       </c>
-    </row>
-    <row r="54" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B54" s="56" t="s">
+      <c r="K53" s="118"/>
+      <c r="L53" s="100"/>
+    </row>
+    <row r="54" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B54" s="140" t="s">
         <v>64</v>
       </c>
-      <c r="C54" s="57"/>
-      <c r="D54" s="58">
+      <c r="C54" s="43"/>
+      <c r="D54" s="44">
         <f>SUM(D48:D53)</f>
-        <v>0.95000000000000007</v>
-      </c>
-      <c r="E54" s="58">
+        <v>0.97000000000000008</v>
+      </c>
+      <c r="E54" s="44">
         <f>SUM(E48:E53)</f>
         <v>0.95000000000000007</v>
       </c>
-      <c r="F54" s="58">
+      <c r="F54" s="44">
         <f>SUM(F48:F53)</f>
         <v>0.95</v>
       </c>
-      <c r="G54" s="58">
+      <c r="G54" s="44">
         <f>SUM(G48:G53)</f>
         <v>0.95</v>
       </c>
-      <c r="H54" s="121">
-        <f>SUM(H48:H53)</f>
-        <v>0.95</v>
-      </c>
-      <c r="I54" s="109">
+      <c r="H54" s="123">
+        <v>95</v>
+      </c>
+      <c r="I54" s="64">
         <f>SUM(J48:J53)</f>
-        <v>0.93740000000000001</v>
-      </c>
-      <c r="J54" s="110"/>
-    </row>
-    <row r="55" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B55" s="28"/>
-      <c r="C55" s="12" t="s">
+        <v>0.95700000000000007</v>
+      </c>
+      <c r="J54" s="65"/>
+      <c r="K54" s="94"/>
+      <c r="L54" s="107"/>
+    </row>
+    <row r="55" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B55" s="136"/>
+      <c r="C55" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="D55" s="29"/>
-      <c r="E55" s="29"/>
-      <c r="F55" s="29"/>
-      <c r="G55" s="112"/>
-      <c r="H55" s="112"/>
-      <c r="I55" s="112"/>
-      <c r="J55" s="111"/>
-    </row>
-    <row r="56" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B56" s="64">
+      <c r="D55" s="20"/>
+      <c r="E55" s="20"/>
+      <c r="F55" s="20"/>
+      <c r="G55" s="68"/>
+      <c r="H55" s="68"/>
+      <c r="I55" s="68"/>
+      <c r="J55" s="69"/>
+      <c r="K55" s="94"/>
+      <c r="L55" s="108"/>
+    </row>
+    <row r="56" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B56" s="144">
         <v>6</v>
       </c>
-      <c r="C56" s="30" t="s">
+      <c r="C56" s="130" t="s">
         <v>51</v>
       </c>
-      <c r="D56" s="40">
-        <v>0.1</v>
-      </c>
-      <c r="E56" s="40">
-        <v>0.1</v>
-      </c>
-      <c r="F56" s="17">
-        <v>0.1</v>
-      </c>
-      <c r="G56" s="35">
-        <v>0.1</v>
-      </c>
-      <c r="H56" s="100">
+      <c r="D56" s="29">
+        <v>0.1</v>
+      </c>
+      <c r="E56" s="29">
+        <v>0.1</v>
+      </c>
+      <c r="F56" s="12">
+        <v>0.1</v>
+      </c>
+      <c r="G56" s="24">
+        <v>0.1</v>
+      </c>
+      <c r="H56" s="55">
         <v>0.15</v>
       </c>
-      <c r="I56" s="97">
+      <c r="I56" s="53">
         <v>0.99</v>
       </c>
-      <c r="J56" s="106">
+      <c r="J56" s="101">
         <f>D56*I56</f>
         <v>9.9000000000000005E-2</v>
       </c>
-    </row>
-    <row r="57" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B57" s="65"/>
-      <c r="C57" s="18" t="s">
+      <c r="K56" s="116">
+        <v>15</v>
+      </c>
+      <c r="L56" s="98">
+        <f>H63*K56/100</f>
+        <v>14.25</v>
+      </c>
+    </row>
+    <row r="57" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B57" s="145"/>
+      <c r="C57" s="131" t="s">
         <v>52</v>
       </c>
-      <c r="D57" s="41">
-        <v>0.2</v>
-      </c>
-      <c r="E57" s="41">
-        <v>0.1</v>
-      </c>
-      <c r="F57" s="27">
-        <v>0.1</v>
-      </c>
-      <c r="G57" s="27">
-        <v>0.1</v>
-      </c>
-      <c r="H57" s="101">
+      <c r="D57" s="30">
+        <v>0.2</v>
+      </c>
+      <c r="E57" s="30">
+        <v>0.1</v>
+      </c>
+      <c r="F57" s="19">
+        <v>0.1</v>
+      </c>
+      <c r="G57" s="19">
+        <v>0.1</v>
+      </c>
+      <c r="H57" s="56">
         <v>0.15</v>
       </c>
-      <c r="I57" s="95">
+      <c r="I57" s="52">
         <v>1</v>
       </c>
-      <c r="J57" s="106">
+      <c r="J57" s="101">
         <f t="shared" ref="J57:J62" si="4">D57*I57</f>
         <v>0.2</v>
       </c>
-    </row>
-    <row r="58" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B58" s="65"/>
-      <c r="C58" s="18" t="s">
+      <c r="K57" s="117"/>
+      <c r="L57" s="99"/>
+    </row>
+    <row r="58" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B58" s="145"/>
+      <c r="C58" s="131" t="s">
         <v>53</v>
       </c>
-      <c r="D58" s="41">
-        <v>0.2</v>
-      </c>
-      <c r="E58" s="41">
-        <v>0.2</v>
-      </c>
-      <c r="F58" s="27">
-        <v>0.1</v>
-      </c>
-      <c r="G58" s="27">
-        <v>0.1</v>
-      </c>
-      <c r="H58" s="101">
+      <c r="D58" s="30">
+        <v>0.2</v>
+      </c>
+      <c r="E58" s="30">
+        <v>0.2</v>
+      </c>
+      <c r="F58" s="19">
+        <v>0.1</v>
+      </c>
+      <c r="G58" s="19">
+        <v>0.1</v>
+      </c>
+      <c r="H58" s="56">
         <v>0.15</v>
       </c>
-      <c r="I58" s="95">
+      <c r="I58" s="52">
         <v>1</v>
       </c>
-      <c r="J58" s="106">
+      <c r="J58" s="101">
         <f t="shared" si="4"/>
         <v>0.2</v>
       </c>
-    </row>
-    <row r="59" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B59" s="65"/>
-      <c r="C59" s="18" t="s">
+      <c r="K58" s="117"/>
+      <c r="L58" s="99"/>
+    </row>
+    <row r="59" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B59" s="145"/>
+      <c r="C59" s="131" t="s">
         <v>54</v>
       </c>
-      <c r="D59" s="41">
-        <v>0.1</v>
-      </c>
-      <c r="E59" s="41">
+      <c r="D59" s="30">
+        <v>0.1</v>
+      </c>
+      <c r="E59" s="30">
         <v>0.15</v>
       </c>
-      <c r="F59" s="27">
+      <c r="F59" s="19">
         <v>0.05</v>
       </c>
-      <c r="G59" s="27">
+      <c r="G59" s="19">
         <v>0.05</v>
       </c>
-      <c r="H59" s="101">
-        <v>0.1</v>
-      </c>
-      <c r="I59" s="95">
+      <c r="H59" s="56">
+        <v>0.1</v>
+      </c>
+      <c r="I59" s="52">
         <v>1</v>
       </c>
-      <c r="J59" s="106">
+      <c r="J59" s="101">
         <f t="shared" si="4"/>
         <v>0.1</v>
       </c>
-    </row>
-    <row r="60" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B60" s="65"/>
-      <c r="C60" s="18" t="s">
+      <c r="K59" s="117"/>
+      <c r="L59" s="99"/>
+    </row>
+    <row r="60" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B60" s="145"/>
+      <c r="C60" s="131" t="s">
         <v>55</v>
       </c>
-      <c r="D60" s="41">
-        <v>0.1</v>
-      </c>
-      <c r="E60" s="41">
-        <v>0.2</v>
-      </c>
-      <c r="F60" s="27">
-        <v>0.1</v>
-      </c>
-      <c r="G60" s="27">
-        <v>0.1</v>
-      </c>
-      <c r="H60" s="101">
+      <c r="D60" s="30">
+        <v>0.1</v>
+      </c>
+      <c r="E60" s="30">
+        <v>0.2</v>
+      </c>
+      <c r="F60" s="19">
+        <v>0.1</v>
+      </c>
+      <c r="G60" s="19">
+        <v>0.1</v>
+      </c>
+      <c r="H60" s="56">
         <v>0.15</v>
       </c>
-      <c r="I60" s="95">
+      <c r="I60" s="52">
         <v>1</v>
       </c>
-      <c r="J60" s="106">
+      <c r="J60" s="101">
         <f t="shared" si="4"/>
         <v>0.1</v>
       </c>
-    </row>
-    <row r="61" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B61" s="65"/>
-      <c r="C61" s="18" t="s">
+      <c r="K60" s="117"/>
+      <c r="L60" s="99"/>
+    </row>
+    <row r="61" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B61" s="145"/>
+      <c r="C61" s="131" t="s">
         <v>56</v>
       </c>
-      <c r="D61" s="41">
-        <v>0.1</v>
-      </c>
-      <c r="E61" s="41">
-        <v>0.1</v>
-      </c>
-      <c r="F61" s="27">
+      <c r="D61" s="30">
+        <v>0.1</v>
+      </c>
+      <c r="E61" s="30">
+        <v>0.1</v>
+      </c>
+      <c r="F61" s="19">
         <v>0.4</v>
       </c>
-      <c r="G61" s="27">
-        <v>0.1</v>
-      </c>
-      <c r="H61" s="101">
+      <c r="G61" s="19">
+        <v>0.1</v>
+      </c>
+      <c r="H61" s="56">
         <v>0.15</v>
       </c>
-      <c r="I61" s="95">
+      <c r="I61" s="52">
         <v>1</v>
       </c>
-      <c r="J61" s="106">
+      <c r="J61" s="101">
         <f t="shared" si="4"/>
         <v>0.1</v>
       </c>
-    </row>
-    <row r="62" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B62" s="66"/>
-      <c r="C62" s="31" t="s">
+      <c r="K61" s="117"/>
+      <c r="L61" s="99"/>
+    </row>
+    <row r="62" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B62" s="146"/>
+      <c r="C62" s="132" t="s">
         <v>57</v>
       </c>
-      <c r="D62" s="37">
-        <v>0.15</v>
-      </c>
-      <c r="E62" s="37">
-        <v>0.1</v>
-      </c>
-      <c r="F62" s="27">
-        <v>0.1</v>
-      </c>
-      <c r="G62" s="27">
+      <c r="D62" s="26">
+        <v>0.2</v>
+      </c>
+      <c r="E62" s="26">
+        <v>0.1</v>
+      </c>
+      <c r="F62" s="19">
+        <v>0.1</v>
+      </c>
+      <c r="G62" s="19">
         <v>0.4</v>
       </c>
-      <c r="H62" s="101">
-        <v>0.1</v>
-      </c>
-      <c r="I62" s="107">
-        <v>0.99</v>
-      </c>
-      <c r="J62" s="106">
+      <c r="H62" s="56">
+        <v>0.1</v>
+      </c>
+      <c r="I62" s="58">
+        <v>0.98</v>
+      </c>
+      <c r="J62" s="101">
         <f t="shared" si="4"/>
-        <v>0.14849999999999999</v>
-      </c>
-    </row>
-    <row r="63" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B63" s="56" t="s">
+        <v>0.19600000000000001</v>
+      </c>
+      <c r="K62" s="118"/>
+      <c r="L62" s="100"/>
+    </row>
+    <row r="63" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B63" s="140" t="s">
         <v>64</v>
       </c>
-      <c r="C63" s="57"/>
-      <c r="D63" s="58">
+      <c r="C63" s="43"/>
+      <c r="D63" s="44">
         <f>SUM(D56:D62)</f>
-        <v>0.95</v>
-      </c>
-      <c r="E63" s="58">
+        <v>1</v>
+      </c>
+      <c r="E63" s="44">
         <f>SUM(E56:E62)</f>
         <v>0.95</v>
       </c>
-      <c r="F63" s="58">
+      <c r="F63" s="44">
         <f>SUM(F56:F62)</f>
         <v>0.95000000000000007</v>
       </c>
-      <c r="G63" s="58">
+      <c r="G63" s="44">
         <f>SUM(G56:G62)</f>
         <v>0.95000000000000007</v>
       </c>
-      <c r="H63" s="121">
-        <f>SUM(H56:H62)</f>
-        <v>0.95</v>
-      </c>
-      <c r="I63" s="109">
+      <c r="H63" s="123">
+        <v>95</v>
+      </c>
+      <c r="I63" s="64">
         <f>SUM(J56:J62)</f>
-        <v>0.94750000000000001</v>
-      </c>
-      <c r="J63" s="110"/>
-    </row>
-    <row r="64" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B64" s="28"/>
-      <c r="C64" s="25" t="s">
+        <v>0.99500000000000011</v>
+      </c>
+      <c r="J63" s="65"/>
+      <c r="K63" s="94"/>
+      <c r="L63" s="107"/>
+    </row>
+    <row r="64" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B64" s="136"/>
+      <c r="C64" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="D64" s="29"/>
-      <c r="E64" s="29"/>
-      <c r="F64" s="29"/>
-      <c r="G64" s="29"/>
-      <c r="H64" s="113"/>
-      <c r="I64" s="114"/>
-      <c r="J64" s="115"/>
-    </row>
-    <row r="65" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B65" s="67">
+      <c r="D64" s="20"/>
+      <c r="E64" s="20"/>
+      <c r="F64" s="20"/>
+      <c r="G64" s="20"/>
+      <c r="H64" s="59"/>
+      <c r="I64" s="60"/>
+      <c r="J64" s="61"/>
+      <c r="K64" s="94"/>
+      <c r="L64" s="108"/>
+    </row>
+    <row r="65" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B65" s="141">
         <v>7</v>
       </c>
-      <c r="C65" s="30" t="s">
+      <c r="C65" s="130" t="s">
         <v>59</v>
       </c>
-      <c r="D65" s="19">
+      <c r="D65" s="13">
+        <v>0.2</v>
+      </c>
+      <c r="E65" s="13">
         <v>0.15</v>
       </c>
-      <c r="E65" s="19">
+      <c r="F65" s="12">
         <v>0.15</v>
       </c>
-      <c r="F65" s="17">
+      <c r="G65" s="12">
         <v>0.15</v>
       </c>
-      <c r="G65" s="17">
+      <c r="H65" s="51">
         <v>0.15</v>
       </c>
-      <c r="H65" s="94">
-        <v>0.15</v>
-      </c>
-      <c r="I65" s="97">
+      <c r="I65" s="53">
         <v>0.99</v>
       </c>
-      <c r="J65" s="106">
+      <c r="J65" s="101">
         <f>D65*I65</f>
-        <v>0.14849999999999999</v>
-      </c>
-    </row>
-    <row r="66" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B66" s="68"/>
-      <c r="C66" s="18" t="s">
+        <v>0.19800000000000001</v>
+      </c>
+      <c r="K65" s="116">
+        <v>10</v>
+      </c>
+      <c r="L65" s="98">
+        <f>H70*K65/100</f>
+        <v>9.5</v>
+      </c>
+    </row>
+    <row r="66" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B66" s="142"/>
+      <c r="C66" s="131" t="s">
         <v>0</v>
       </c>
-      <c r="D66" s="52">
-        <v>0.2</v>
-      </c>
-      <c r="E66" s="19">
-        <v>0.2</v>
-      </c>
-      <c r="F66" s="19">
-        <v>0.2</v>
-      </c>
-      <c r="G66" s="19">
-        <v>0.2</v>
-      </c>
-      <c r="H66" s="118">
-        <v>0.2</v>
-      </c>
-      <c r="I66" s="95">
+      <c r="D66" s="40">
+        <v>0.2</v>
+      </c>
+      <c r="E66" s="13">
+        <v>0.2</v>
+      </c>
+      <c r="F66" s="13">
+        <v>0.2</v>
+      </c>
+      <c r="G66" s="13">
+        <v>0.2</v>
+      </c>
+      <c r="H66" s="62">
+        <v>0.2</v>
+      </c>
+      <c r="I66" s="52">
         <v>0.99</v>
       </c>
-      <c r="J66" s="106">
+      <c r="J66" s="101">
         <f t="shared" ref="J66:J69" si="5">D66*I66</f>
         <v>0.19800000000000001</v>
       </c>
-    </row>
-    <row r="67" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B67" s="68"/>
-      <c r="C67" s="31" t="s">
+      <c r="K66" s="117"/>
+      <c r="L66" s="99"/>
+    </row>
+    <row r="67" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B67" s="142"/>
+      <c r="C67" s="132" t="s">
         <v>16</v>
       </c>
-      <c r="D67" s="52">
-        <v>0.2</v>
-      </c>
-      <c r="E67" s="52">
-        <v>0.2</v>
-      </c>
-      <c r="F67" s="22">
-        <v>0.2</v>
-      </c>
-      <c r="G67" s="22">
-        <v>0.2</v>
-      </c>
-      <c r="H67" s="101">
-        <v>0.2</v>
-      </c>
-      <c r="I67" s="95">
+      <c r="D67" s="40">
+        <v>0.2</v>
+      </c>
+      <c r="E67" s="40">
+        <v>0.2</v>
+      </c>
+      <c r="F67" s="15">
+        <v>0.2</v>
+      </c>
+      <c r="G67" s="15">
+        <v>0.2</v>
+      </c>
+      <c r="H67" s="56">
+        <v>0.2</v>
+      </c>
+      <c r="I67" s="52">
         <v>0.99</v>
       </c>
-      <c r="J67" s="106">
+      <c r="J67" s="101">
         <f t="shared" si="5"/>
         <v>0.19800000000000001</v>
       </c>
-    </row>
-    <row r="68" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B68" s="68"/>
-      <c r="C68" s="51" t="s">
+      <c r="K67" s="117"/>
+      <c r="L67" s="99"/>
+    </row>
+    <row r="68" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B68" s="142"/>
+      <c r="C68" s="133" t="s">
         <v>71</v>
       </c>
-      <c r="D68" s="52">
-        <v>0.2</v>
-      </c>
-      <c r="E68" s="52">
-        <v>0.2</v>
-      </c>
-      <c r="F68" s="22">
-        <v>0.2</v>
-      </c>
-      <c r="G68" s="22">
-        <v>0.2</v>
-      </c>
-      <c r="H68" s="101">
-        <v>0.2</v>
-      </c>
-      <c r="I68" s="95">
+      <c r="D68" s="40">
+        <v>0.2</v>
+      </c>
+      <c r="E68" s="40">
+        <v>0.2</v>
+      </c>
+      <c r="F68" s="15">
+        <v>0.2</v>
+      </c>
+      <c r="G68" s="15">
+        <v>0.2</v>
+      </c>
+      <c r="H68" s="56">
+        <v>0.2</v>
+      </c>
+      <c r="I68" s="52">
         <v>0.99</v>
       </c>
-      <c r="J68" s="106">
+      <c r="J68" s="101">
         <f t="shared" si="5"/>
         <v>0.19800000000000001</v>
       </c>
-    </row>
-    <row r="69" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B69" s="68"/>
-      <c r="C69" s="31" t="s">
+      <c r="K68" s="117"/>
+      <c r="L68" s="99"/>
+    </row>
+    <row r="69" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B69" s="143"/>
+      <c r="C69" s="132" t="s">
         <v>72</v>
       </c>
-      <c r="D69" s="27">
-        <v>0.2</v>
-      </c>
-      <c r="E69" s="27">
-        <v>0.2</v>
-      </c>
-      <c r="F69" s="22">
-        <v>0.2</v>
-      </c>
-      <c r="G69" s="22">
-        <v>0.2</v>
-      </c>
-      <c r="H69" s="101">
-        <v>0.2</v>
-      </c>
-      <c r="I69" s="107">
+      <c r="D69" s="19">
+        <v>0.2</v>
+      </c>
+      <c r="E69" s="19">
+        <v>0.2</v>
+      </c>
+      <c r="F69" s="15">
+        <v>0.2</v>
+      </c>
+      <c r="G69" s="15">
+        <v>0.2</v>
+      </c>
+      <c r="H69" s="56">
+        <v>0.2</v>
+      </c>
+      <c r="I69" s="58">
         <v>0.99</v>
       </c>
-      <c r="J69" s="106">
+      <c r="J69" s="101">
         <f t="shared" si="5"/>
         <v>0.19800000000000001</v>
       </c>
-    </row>
-    <row r="70" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B70" s="53" t="s">
+      <c r="K69" s="118"/>
+      <c r="L69" s="100"/>
+    </row>
+    <row r="70" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B70" s="139" t="s">
         <v>64</v>
       </c>
-      <c r="C70" s="54"/>
-      <c r="D70" s="55">
+      <c r="C70" s="41"/>
+      <c r="D70" s="42">
         <f>SUM(D65:D69)</f>
-        <v>0.95</v>
-      </c>
-      <c r="E70" s="55">
+        <v>1</v>
+      </c>
+      <c r="E70" s="42">
         <f>SUM(E65:E69)</f>
         <v>0.95</v>
       </c>
-      <c r="F70" s="55">
+      <c r="F70" s="42">
         <f>SUM(F65:F69)</f>
         <v>0.95</v>
       </c>
-      <c r="G70" s="55">
+      <c r="G70" s="42">
         <f>SUM(G65:G69)</f>
         <v>0.95</v>
       </c>
-      <c r="H70" s="119">
-        <f>SUM(H65:H69)</f>
-        <v>0.95</v>
-      </c>
-      <c r="I70" s="104">
+      <c r="H70" s="124">
+        <v>95</v>
+      </c>
+      <c r="I70" s="66">
         <f>SUM(J65:J69)</f>
-        <v>0.94049999999999989</v>
-      </c>
-      <c r="J70" s="105"/>
-    </row>
-    <row r="71" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B71" s="32"/>
-    </row>
-    <row r="72" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B72" s="32"/>
-    </row>
-    <row r="73" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B73" s="32"/>
-    </row>
-    <row r="74" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B74" s="32"/>
-    </row>
-    <row r="75" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B75" s="32"/>
-    </row>
-    <row r="76" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B76" s="32"/>
-    </row>
-    <row r="77" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B77" s="32"/>
-    </row>
-    <row r="78" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B78" s="32"/>
-    </row>
-    <row r="79" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B79" s="32"/>
-    </row>
-    <row r="80" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B80" s="32"/>
+        <v>0.99</v>
+      </c>
+      <c r="J70" s="67"/>
+      <c r="K70" s="94"/>
+      <c r="L70" s="94"/>
+    </row>
+    <row r="71" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B71" s="21"/>
+      <c r="I71" s="93"/>
+      <c r="K71" s="125">
+        <f>SUM(K20,K33,K41,K48,K56,K65)</f>
+        <v>100</v>
+      </c>
+      <c r="L71" s="126">
+        <f>SUM(L20,L33,L41,L48,L56,L65)</f>
+        <v>95.9</v>
+      </c>
+    </row>
+    <row r="72" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B72" s="21"/>
+    </row>
+    <row r="73" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B73" s="21"/>
+    </row>
+    <row r="74" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B74" s="21"/>
+    </row>
+    <row r="75" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B75" s="21"/>
+    </row>
+    <row r="76" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B76" s="21"/>
+    </row>
+    <row r="77" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B77" s="21"/>
+    </row>
+    <row r="78" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B78" s="21"/>
+    </row>
+    <row r="79" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B79" s="21"/>
+    </row>
+    <row r="80" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B80" s="21"/>
     </row>
     <row r="81" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B81" s="32"/>
+      <c r="B81" s="21"/>
     </row>
     <row r="82" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B82" s="32"/>
+      <c r="B82" s="21"/>
     </row>
     <row r="83" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B83" s="32"/>
+      <c r="B83" s="21"/>
     </row>
     <row r="84" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B84" s="32"/>
+      <c r="B84" s="21"/>
     </row>
     <row r="85" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B85" s="32"/>
+      <c r="B85" s="21"/>
     </row>
     <row r="86" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B86" s="32"/>
+      <c r="B86" s="21"/>
     </row>
     <row r="87" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B87" s="32"/>
+      <c r="B87" s="21"/>
     </row>
     <row r="88" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B88" s="32"/>
+      <c r="B88" s="21"/>
     </row>
     <row r="89" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B89" s="32"/>
+      <c r="B89" s="21"/>
     </row>
     <row r="90" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B90" s="32"/>
+      <c r="B90" s="21"/>
     </row>
     <row r="91" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B91" s="32"/>
+      <c r="B91" s="21"/>
     </row>
     <row r="92" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B92" s="32"/>
+      <c r="B92" s="21"/>
     </row>
     <row r="93" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B93" s="32"/>
+      <c r="B93" s="21"/>
     </row>
     <row r="94" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B94" s="32"/>
+      <c r="B94" s="21"/>
     </row>
     <row r="95" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B95" s="32"/>
+      <c r="B95" s="21"/>
     </row>
     <row r="96" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B96" s="32"/>
+      <c r="B96" s="21"/>
     </row>
     <row r="97" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B97" s="32"/>
+      <c r="B97" s="21"/>
     </row>
     <row r="98" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B98" s="32"/>
+      <c r="B98" s="21"/>
     </row>
     <row r="99" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B99" s="32"/>
+      <c r="B99" s="21"/>
     </row>
     <row r="100" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B100" s="32"/>
+      <c r="B100" s="21"/>
     </row>
     <row r="101" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B101" s="32"/>
+      <c r="B101" s="21"/>
     </row>
     <row r="102" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B102" s="32"/>
+      <c r="B102" s="21"/>
     </row>
     <row r="103" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B103" s="32"/>
+      <c r="B103" s="21"/>
     </row>
     <row r="104" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B104" s="32"/>
+      <c r="B104" s="21"/>
     </row>
     <row r="105" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B105" s="32"/>
+      <c r="B105" s="21"/>
     </row>
     <row r="106" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B106" s="32"/>
+      <c r="B106" s="21"/>
     </row>
     <row r="107" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B107" s="32"/>
+      <c r="B107" s="21"/>
     </row>
     <row r="108" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B108" s="32"/>
+      <c r="B108" s="21"/>
     </row>
     <row r="109" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B109" s="32"/>
+      <c r="B109" s="21"/>
     </row>
     <row r="110" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B110" s="32"/>
+      <c r="B110" s="21"/>
     </row>
     <row r="111" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B111" s="32"/>
+      <c r="B111" s="21"/>
     </row>
     <row r="112" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B112" s="32"/>
+      <c r="B112" s="21"/>
     </row>
     <row r="113" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B113" s="32"/>
+      <c r="B113" s="21"/>
     </row>
     <row r="114" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B114" s="32"/>
+      <c r="B114" s="21"/>
     </row>
     <row r="115" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B115" s="32"/>
+      <c r="B115" s="21"/>
     </row>
     <row r="116" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B116" s="32"/>
+      <c r="B116" s="21"/>
     </row>
     <row r="117" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B117" s="32"/>
+      <c r="B117" s="21"/>
     </row>
     <row r="118" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B118" s="32"/>
+      <c r="B118" s="21"/>
     </row>
     <row r="119" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B119" s="32"/>
+      <c r="B119" s="21"/>
     </row>
     <row r="120" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B120" s="32"/>
+      <c r="B120" s="21"/>
     </row>
     <row r="121" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B121" s="32"/>
+      <c r="B121" s="21"/>
     </row>
     <row r="122" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B122" s="32"/>
+      <c r="B122" s="21"/>
     </row>
     <row r="123" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B123" s="32"/>
+      <c r="B123" s="21"/>
     </row>
     <row r="124" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B124" s="32"/>
+      <c r="B124" s="21"/>
     </row>
     <row r="125" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B125" s="32"/>
+      <c r="B125" s="21"/>
     </row>
     <row r="126" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B126" s="32"/>
+      <c r="B126" s="21"/>
     </row>
     <row r="127" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B127" s="32"/>
+      <c r="B127" s="21"/>
     </row>
     <row r="128" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B128" s="32"/>
+      <c r="B128" s="21"/>
     </row>
     <row r="129" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B129" s="32"/>
+      <c r="B129" s="21"/>
     </row>
     <row r="130" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B130" s="32"/>
+      <c r="B130" s="21"/>
     </row>
     <row r="131" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B131" s="32"/>
+      <c r="B131" s="21"/>
     </row>
     <row r="132" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B132" s="32"/>
+      <c r="B132" s="21"/>
     </row>
     <row r="133" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B133" s="32"/>
+      <c r="B133" s="21"/>
     </row>
     <row r="134" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B134" s="32"/>
+      <c r="B134" s="21"/>
     </row>
     <row r="135" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B135" s="32"/>
+      <c r="B135" s="21"/>
     </row>
     <row r="136" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B136" s="32"/>
+      <c r="B136" s="21"/>
     </row>
     <row r="137" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B137" s="32"/>
+      <c r="B137" s="21"/>
     </row>
     <row r="138" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B138" s="32"/>
+      <c r="B138" s="21"/>
     </row>
     <row r="139" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B139" s="32"/>
+      <c r="B139" s="21"/>
     </row>
     <row r="140" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B140" s="32"/>
+      <c r="B140" s="21"/>
     </row>
     <row r="141" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B141" s="32"/>
+      <c r="B141" s="21"/>
     </row>
     <row r="142" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B142" s="32"/>
+      <c r="B142" s="21"/>
     </row>
     <row r="143" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B143" s="32"/>
+      <c r="B143" s="21"/>
     </row>
     <row r="144" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B144" s="32"/>
+      <c r="B144" s="21"/>
     </row>
     <row r="145" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B145" s="32"/>
+      <c r="B145" s="21"/>
     </row>
     <row r="146" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B146" s="32"/>
+      <c r="B146" s="21"/>
     </row>
     <row r="147" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B147" s="32"/>
+      <c r="B147" s="21"/>
     </row>
     <row r="148" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B148" s="32"/>
+      <c r="B148" s="21"/>
     </row>
     <row r="149" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B149" s="32"/>
+      <c r="B149" s="21"/>
     </row>
     <row r="150" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B150" s="32"/>
+      <c r="B150" s="21"/>
     </row>
     <row r="151" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B151" s="32"/>
+      <c r="B151" s="21"/>
     </row>
     <row r="152" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B152" s="32"/>
+      <c r="B152" s="21"/>
     </row>
     <row r="1048570" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D1048570" s="17"/>
+      <c r="D1048570" s="12"/>
     </row>
   </sheetData>
-  <mergeCells count="24">
+  <mergeCells count="42">
+    <mergeCell ref="K41:K45"/>
+    <mergeCell ref="K48:K53"/>
+    <mergeCell ref="K56:K62"/>
+    <mergeCell ref="K65:K69"/>
+    <mergeCell ref="L20:L30"/>
+    <mergeCell ref="L31:L32"/>
+    <mergeCell ref="K31:K32"/>
+    <mergeCell ref="L33:L38"/>
+    <mergeCell ref="L39:L40"/>
+    <mergeCell ref="L41:L45"/>
+    <mergeCell ref="L46:L47"/>
+    <mergeCell ref="L48:L53"/>
+    <mergeCell ref="L54:L55"/>
+    <mergeCell ref="L56:L62"/>
+    <mergeCell ref="L63:L64"/>
+    <mergeCell ref="L65:L69"/>
+    <mergeCell ref="I31:J31"/>
+    <mergeCell ref="F32:J32"/>
+    <mergeCell ref="I39:J39"/>
+    <mergeCell ref="K20:K30"/>
+    <mergeCell ref="K33:K38"/>
+    <mergeCell ref="B56:B62"/>
+    <mergeCell ref="B65:B69"/>
+    <mergeCell ref="C13:F13"/>
+    <mergeCell ref="B25:B30"/>
+    <mergeCell ref="B33:B38"/>
+    <mergeCell ref="B41:B45"/>
+    <mergeCell ref="B48:B53"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D3:F10"/>
+    <mergeCell ref="C11:F11"/>
+    <mergeCell ref="C12:F12"/>
+    <mergeCell ref="B20:B24"/>
+    <mergeCell ref="D17:J17"/>
     <mergeCell ref="I54:J54"/>
     <mergeCell ref="I63:J63"/>
     <mergeCell ref="I70:J70"/>
@@ -3782,22 +4103,6 @@
     <mergeCell ref="G47:J47"/>
     <mergeCell ref="I46:J46"/>
     <mergeCell ref="D47:F47"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="D3:F10"/>
-    <mergeCell ref="C11:F11"/>
-    <mergeCell ref="C12:F12"/>
-    <mergeCell ref="B20:B24"/>
-    <mergeCell ref="D17:J17"/>
-    <mergeCell ref="B56:B62"/>
-    <mergeCell ref="B65:B69"/>
-    <mergeCell ref="C13:F13"/>
-    <mergeCell ref="B25:B30"/>
-    <mergeCell ref="B33:B38"/>
-    <mergeCell ref="B41:B45"/>
-    <mergeCell ref="B48:B53"/>
-    <mergeCell ref="I31:J31"/>
-    <mergeCell ref="F32:J32"/>
-    <mergeCell ref="I39:J39"/>
   </mergeCells>
   <conditionalFormatting sqref="D20:D30">
     <cfRule type="colorScale" priority="17">

</xml_diff>